<commit_message>
Updated data sets, but missing 1 student
</commit_message>
<xml_diff>
--- a/data/raw/student_dem_raw.xlsx
+++ b/data/raw/student_dem_raw.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27927"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\LIZ\WiSTEM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sylviaboguniecki/Desktop/wistem_23_24/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{16CA9E1B-09E1-41CD-B6D7-5201256D9CAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{256D63D9-FA55-EC4A-AF0B-17AE8D78029D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{C7C2B227-BBDA-4416-93C7-10628C12C90F}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="19420" windowHeight="16720" xr2:uid="{C7C2B227-BBDA-4416-93C7-10628C12C90F}"/>
   </bookViews>
   <sheets>
     <sheet name="wistem" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1111" uniqueCount="529">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1455" uniqueCount="603">
   <si>
     <t>ID</t>
   </si>
@@ -1623,6 +1623,228 @@
   </si>
   <si>
     <t>Larkin</t>
+  </si>
+  <si>
+    <t>Izzah</t>
+  </si>
+  <si>
+    <t>Shah</t>
+  </si>
+  <si>
+    <t>Frajman</t>
+  </si>
+  <si>
+    <t>Shaili</t>
+  </si>
+  <si>
+    <t>Peters</t>
+  </si>
+  <si>
+    <t>Buell</t>
+  </si>
+  <si>
+    <t>Freeman</t>
+  </si>
+  <si>
+    <t>Rivka</t>
+  </si>
+  <si>
+    <t>Mordka</t>
+  </si>
+  <si>
+    <t>Natalya</t>
+  </si>
+  <si>
+    <t>Kayla</t>
+  </si>
+  <si>
+    <t>Rodriguez</t>
+  </si>
+  <si>
+    <t>Ingrid</t>
+  </si>
+  <si>
+    <t>Olko</t>
+  </si>
+  <si>
+    <t>Sophie</t>
+  </si>
+  <si>
+    <t>Kegler</t>
+  </si>
+  <si>
+    <t>Luenonie Ruvikk</t>
+  </si>
+  <si>
+    <t>Villaruel</t>
+  </si>
+  <si>
+    <t>Gallo</t>
+  </si>
+  <si>
+    <t>Eleanor</t>
+  </si>
+  <si>
+    <t>Feeney</t>
+  </si>
+  <si>
+    <t>Casey</t>
+  </si>
+  <si>
+    <t>Mcdermott</t>
+  </si>
+  <si>
+    <t>Lindsey</t>
+  </si>
+  <si>
+    <t>Cameron</t>
+  </si>
+  <si>
+    <t>Corbett</t>
+  </si>
+  <si>
+    <t>American Indian or Alaska Native</t>
+  </si>
+  <si>
+    <t>Clara</t>
+  </si>
+  <si>
+    <t>Makeda</t>
+  </si>
+  <si>
+    <t>Hausman</t>
+  </si>
+  <si>
+    <t>Leah</t>
+  </si>
+  <si>
+    <t>Amromin</t>
+  </si>
+  <si>
+    <t>Frances</t>
+  </si>
+  <si>
+    <t>Wade</t>
+  </si>
+  <si>
+    <t>Jessica</t>
+  </si>
+  <si>
+    <t>Frolichstein</t>
+  </si>
+  <si>
+    <t>Oaklyn</t>
+  </si>
+  <si>
+    <t>Waldron</t>
+  </si>
+  <si>
+    <t>Solar</t>
+  </si>
+  <si>
+    <t>Alondra</t>
+  </si>
+  <si>
+    <t>Lagunilla</t>
+  </si>
+  <si>
+    <t>Eliza</t>
+  </si>
+  <si>
+    <t>Hogan</t>
+  </si>
+  <si>
+    <t>Vanya</t>
+  </si>
+  <si>
+    <t>Gojakovic</t>
+  </si>
+  <si>
+    <t>Amiah</t>
+  </si>
+  <si>
+    <t>Stringer</t>
+  </si>
+  <si>
+    <t>Martin</t>
+  </si>
+  <si>
+    <t>Susannah</t>
+  </si>
+  <si>
+    <t>Keller</t>
+  </si>
+  <si>
+    <t>Penelope</t>
+  </si>
+  <si>
+    <t>Cohn</t>
+  </si>
+  <si>
+    <t>Quail</t>
+  </si>
+  <si>
+    <t>Harris</t>
+  </si>
+  <si>
+    <t>Vivian</t>
+  </si>
+  <si>
+    <t>Solomon</t>
+  </si>
+  <si>
+    <t>Decastro</t>
+  </si>
+  <si>
+    <t>Laissa</t>
+  </si>
+  <si>
+    <t>Vazquez</t>
+  </si>
+  <si>
+    <t>Natalia</t>
+  </si>
+  <si>
+    <t>Acosta</t>
+  </si>
+  <si>
+    <t>Kelen</t>
+  </si>
+  <si>
+    <t>Kasprzycki</t>
+  </si>
+  <si>
+    <t>Phoebe</t>
+  </si>
+  <si>
+    <t>Kimrey</t>
+  </si>
+  <si>
+    <t>Naiyeli</t>
+  </si>
+  <si>
+    <t>Vera</t>
+  </si>
+  <si>
+    <t>Weinert</t>
+  </si>
+  <si>
+    <t>Wittenberg Trubowitz</t>
+  </si>
+  <si>
+    <t>McDonald</t>
+  </si>
+  <si>
+    <t>Schwendener</t>
+  </si>
+  <si>
+    <t>Thalia</t>
+  </si>
+  <si>
+    <t>Molly</t>
+  </si>
+  <si>
+    <t>O'Hare</t>
   </si>
 </sst>
 </file>
@@ -1632,7 +1854,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#0"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -1642,11 +1864,6 @@
     <font>
       <sz val="8"/>
       <color theme="1"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
@@ -1704,7 +1921,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1715,10 +1932,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2053,38 +2271,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03138AD1-97AD-4498-9D2F-72B0C051055A}">
-  <dimension ref="A1:G185"/>
+  <dimension ref="A1:G257"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A229" workbookViewId="0">
+      <selection activeCell="M185" sqref="M185"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.19921875" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="16384" width="9.19921875" style="6"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" ht="12.95" thickBot="1">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="12.95" thickBot="1">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
@@ -2107,7 +2328,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="12.95" thickBot="1">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
         <v>13</v>
       </c>
@@ -2130,7 +2351,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="12.95" thickBot="1">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" s="3" t="s">
         <v>17</v>
       </c>
@@ -2153,7 +2374,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="12.95" thickBot="1">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="3" t="s">
         <v>19</v>
       </c>
@@ -2176,7 +2397,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="12.95" thickBot="1">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" s="3" t="s">
         <v>22</v>
       </c>
@@ -2199,7 +2420,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="12.95" thickBot="1">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A7" s="3" t="s">
         <v>26</v>
       </c>
@@ -2222,7 +2443,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="12.95" thickBot="1">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8" s="3" t="s">
         <v>30</v>
       </c>
@@ -2245,7 +2466,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="12.95" thickBot="1">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A9" s="3" t="s">
         <v>33</v>
       </c>
@@ -2268,7 +2489,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="12.95" thickBot="1">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A10" s="3" t="s">
         <v>36</v>
       </c>
@@ -2291,7 +2512,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="12.95" thickBot="1">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A11" s="3" t="s">
         <v>39</v>
       </c>
@@ -2314,7 +2535,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="12.95" thickBot="1">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A12" s="3" t="s">
         <v>42</v>
       </c>
@@ -2337,7 +2558,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="12.95" thickBot="1">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A13" s="3" t="s">
         <v>45</v>
       </c>
@@ -2360,7 +2581,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="12.95" thickBot="1">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A14" s="3" t="s">
         <v>48</v>
       </c>
@@ -2383,7 +2604,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="12.95" thickBot="1">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A15" s="3" t="s">
         <v>51</v>
       </c>
@@ -2406,7 +2627,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="12.95" thickBot="1">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A16" s="3" t="s">
         <v>54</v>
       </c>
@@ -2429,7 +2650,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="12.95" thickBot="1">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A17" s="3" t="s">
         <v>57</v>
       </c>
@@ -2452,7 +2673,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="12.95" thickBot="1">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A18" s="3" t="s">
         <v>60</v>
       </c>
@@ -2475,7 +2696,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="12.95" thickBot="1">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A19" s="3" t="s">
         <v>63</v>
       </c>
@@ -2498,7 +2719,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="12.95" thickBot="1">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A20" s="3" t="s">
         <v>66</v>
       </c>
@@ -2521,7 +2742,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="12.95" thickBot="1">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A21" s="3" t="s">
         <v>69</v>
       </c>
@@ -2544,7 +2765,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="12.95" thickBot="1">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A22" s="3" t="s">
         <v>73</v>
       </c>
@@ -2567,7 +2788,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="12.95" thickBot="1">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A23" s="3" t="s">
         <v>76</v>
       </c>
@@ -2590,7 +2811,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="12.95" thickBot="1">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A24" s="3" t="s">
         <v>79</v>
       </c>
@@ -2613,7 +2834,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="12.95" thickBot="1">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A25" s="3" t="s">
         <v>82</v>
       </c>
@@ -2636,7 +2857,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="12.95" thickBot="1">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A26" s="3" t="s">
         <v>85</v>
       </c>
@@ -2659,7 +2880,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="12.95" thickBot="1">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A27" s="3" t="s">
         <v>88</v>
       </c>
@@ -2682,7 +2903,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="12.95" thickBot="1">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A28" s="3" t="s">
         <v>90</v>
       </c>
@@ -2705,7 +2926,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="12.95" thickBot="1">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A29" s="3" t="s">
         <v>93</v>
       </c>
@@ -2728,7 +2949,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="12.95" thickBot="1">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A30" s="3" t="s">
         <v>96</v>
       </c>
@@ -2751,7 +2972,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="12.95" thickBot="1">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A31" s="3" t="s">
         <v>99</v>
       </c>
@@ -2774,7 +2995,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="12.95" thickBot="1">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A32" s="3" t="s">
         <v>101</v>
       </c>
@@ -2797,7 +3018,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="12.95" thickBot="1">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A33" s="3" t="s">
         <v>103</v>
       </c>
@@ -2820,7 +3041,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="12.95" thickBot="1">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A34" s="3" t="s">
         <v>106</v>
       </c>
@@ -2843,7 +3064,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="12.95" thickBot="1">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A35" s="3" t="s">
         <v>109</v>
       </c>
@@ -2866,7 +3087,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="12.95" thickBot="1">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A36" s="3" t="s">
         <v>111</v>
       </c>
@@ -2889,7 +3110,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="12.95" thickBot="1">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A37" s="3" t="s">
         <v>114</v>
       </c>
@@ -2912,7 +3133,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="12.95" thickBot="1">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A38" s="3" t="s">
         <v>117</v>
       </c>
@@ -2935,7 +3156,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="12.95" thickBot="1">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A39" s="3" t="s">
         <v>120</v>
       </c>
@@ -2958,7 +3179,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="12.95" thickBot="1">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A40" s="3" t="s">
         <v>123</v>
       </c>
@@ -2981,7 +3202,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="12.95" thickBot="1">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A41" s="3" t="s">
         <v>126</v>
       </c>
@@ -3004,7 +3225,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="12.95" thickBot="1">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A42" s="3" t="s">
         <v>129</v>
       </c>
@@ -3027,7 +3248,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="12.95" thickBot="1">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A43" s="3" t="s">
         <v>132</v>
       </c>
@@ -3050,7 +3271,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="12.95" thickBot="1">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A44" s="3" t="s">
         <v>135</v>
       </c>
@@ -3073,7 +3294,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="12.95" thickBot="1">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A45" s="3" t="s">
         <v>138</v>
       </c>
@@ -3096,7 +3317,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="12.95" thickBot="1">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A46" s="3" t="s">
         <v>140</v>
       </c>
@@ -3119,7 +3340,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="12.95" thickBot="1">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A47" s="3" t="s">
         <v>143</v>
       </c>
@@ -3142,7 +3363,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="12.95" thickBot="1">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A48" s="3" t="s">
         <v>146</v>
       </c>
@@ -3165,7 +3386,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="12.95" thickBot="1">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A49" s="3" t="s">
         <v>148</v>
       </c>
@@ -3188,7 +3409,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="12.95" thickBot="1">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A50" s="3" t="s">
         <v>151</v>
       </c>
@@ -3211,7 +3432,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="12.95" thickBot="1">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A51" s="3" t="s">
         <v>154</v>
       </c>
@@ -3234,7 +3455,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="12.95" thickBot="1">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A52" s="3" t="s">
         <v>157</v>
       </c>
@@ -3257,7 +3478,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="12.95" thickBot="1">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A53" s="3" t="s">
         <v>160</v>
       </c>
@@ -3280,7 +3501,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="12.95" thickBot="1">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A54" s="3" t="s">
         <v>163</v>
       </c>
@@ -3303,7 +3524,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="12.95" thickBot="1">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A55" s="3" t="s">
         <v>166</v>
       </c>
@@ -3326,7 +3547,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="12.95" thickBot="1">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A56" s="3" t="s">
         <v>169</v>
       </c>
@@ -3349,7 +3570,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="12.95" thickBot="1">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A57" s="3" t="s">
         <v>172</v>
       </c>
@@ -3372,7 +3593,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="12.95" thickBot="1">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A58" s="3" t="s">
         <v>175</v>
       </c>
@@ -3395,7 +3616,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="12.95" thickBot="1">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A59" s="3" t="s">
         <v>178</v>
       </c>
@@ -3418,7 +3639,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="12.95" thickBot="1">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A60" s="3" t="s">
         <v>181</v>
       </c>
@@ -3441,7 +3662,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="12.95" thickBot="1">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A61" s="3" t="s">
         <v>184</v>
       </c>
@@ -3464,7 +3685,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="12.95" thickBot="1">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A62" s="3" t="s">
         <v>187</v>
       </c>
@@ -3487,7 +3708,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="12.95" thickBot="1">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A63" s="3" t="s">
         <v>190</v>
       </c>
@@ -3510,7 +3731,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="64" spans="1:7" ht="12.95" thickBot="1">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A64" s="3" t="s">
         <v>193</v>
       </c>
@@ -3533,7 +3754,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="12.95" thickBot="1">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A65" s="3" t="s">
         <v>196</v>
       </c>
@@ -3556,7 +3777,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="66" spans="1:7" ht="12.95" thickBot="1">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A66" s="3" t="s">
         <v>199</v>
       </c>
@@ -3579,7 +3800,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="12.95" thickBot="1">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A67" s="3" t="s">
         <v>202</v>
       </c>
@@ -3602,7 +3823,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="68" spans="1:7" ht="12.95" thickBot="1">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A68" s="3" t="s">
         <v>205</v>
       </c>
@@ -3625,7 +3846,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="69" spans="1:7" ht="12.95" thickBot="1">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A69" s="3" t="s">
         <v>208</v>
       </c>
@@ -3648,7 +3869,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="70" spans="1:7" ht="12.95" thickBot="1">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A70" s="3" t="s">
         <v>211</v>
       </c>
@@ -3671,7 +3892,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="71" spans="1:7" ht="12.95" thickBot="1">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A71" s="3" t="s">
         <v>214</v>
       </c>
@@ -3694,7 +3915,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="72" spans="1:7" ht="12.95" thickBot="1">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A72" s="3" t="s">
         <v>217</v>
       </c>
@@ -3717,7 +3938,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="73" spans="1:7" ht="12.95" thickBot="1">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A73" s="3" t="s">
         <v>219</v>
       </c>
@@ -3740,7 +3961,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="74" spans="1:7" ht="12.95" thickBot="1">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A74" s="3" t="s">
         <v>222</v>
       </c>
@@ -3763,7 +3984,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="75" spans="1:7" ht="12.95" thickBot="1">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A75" s="3" t="s">
         <v>225</v>
       </c>
@@ -3786,7 +4007,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="76" spans="1:7" ht="12.95" thickBot="1">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A76" s="3" t="s">
         <v>227</v>
       </c>
@@ -3809,7 +4030,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="77" spans="1:7" ht="12.95" thickBot="1">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A77" s="3" t="s">
         <v>230</v>
       </c>
@@ -3832,7 +4053,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="78" spans="1:7" ht="12.95" thickBot="1">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A78" s="3" t="s">
         <v>233</v>
       </c>
@@ -3855,7 +4076,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="79" spans="1:7" ht="12.95" thickBot="1">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A79" s="3" t="s">
         <v>236</v>
       </c>
@@ -3878,7 +4099,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="80" spans="1:7" ht="12.95" thickBot="1">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A80" s="3" t="s">
         <v>239</v>
       </c>
@@ -3901,7 +4122,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="81" spans="1:7" ht="12.95" thickBot="1">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A81" s="3" t="s">
         <v>242</v>
       </c>
@@ -3924,7 +4145,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="82" spans="1:7" ht="12.95" thickBot="1">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A82" s="3" t="s">
         <v>245</v>
       </c>
@@ -3947,7 +4168,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="83" spans="1:7" ht="12.95" thickBot="1">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A83" s="3" t="s">
         <v>248</v>
       </c>
@@ -3970,7 +4191,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="84" spans="1:7" ht="12.95" thickBot="1">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A84" s="3" t="s">
         <v>251</v>
       </c>
@@ -3993,7 +4214,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="85" spans="1:7" ht="12.95" thickBot="1">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A85" s="3" t="s">
         <v>254</v>
       </c>
@@ -4016,7 +4237,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="86" spans="1:7" ht="12.95" thickBot="1">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A86" s="3" t="s">
         <v>257</v>
       </c>
@@ -4039,7 +4260,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="87" spans="1:7" ht="12.95" thickBot="1">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A87" s="3" t="s">
         <v>260</v>
       </c>
@@ -4062,7 +4283,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="88" spans="1:7" ht="12.95" thickBot="1">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A88" s="3" t="s">
         <v>263</v>
       </c>
@@ -4085,7 +4306,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="89" spans="1:7" ht="12.95" thickBot="1">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A89" s="3" t="s">
         <v>265</v>
       </c>
@@ -4108,7 +4329,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="90" spans="1:7" ht="12.95" thickBot="1">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A90" s="3" t="s">
         <v>268</v>
       </c>
@@ -4131,7 +4352,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="91" spans="1:7" ht="12.95" thickBot="1">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A91" s="3" t="s">
         <v>271</v>
       </c>
@@ -4154,7 +4375,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="92" spans="1:7" ht="12.95" thickBot="1">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A92" s="3" t="s">
         <v>274</v>
       </c>
@@ -4177,7 +4398,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="93" spans="1:7" ht="12.95" thickBot="1">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A93" s="3" t="s">
         <v>277</v>
       </c>
@@ -4200,7 +4421,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="94" spans="1:7" ht="12.95" thickBot="1">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A94" s="3" t="s">
         <v>280</v>
       </c>
@@ -4223,7 +4444,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="95" spans="1:7" ht="12.95" thickBot="1">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A95" s="3" t="s">
         <v>283</v>
       </c>
@@ -4246,7 +4467,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="96" spans="1:7" ht="12.95" thickBot="1">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A96" s="3" t="s">
         <v>286</v>
       </c>
@@ -4269,7 +4490,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="97" spans="1:7" ht="12.95" thickBot="1">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A97" s="3" t="s">
         <v>289</v>
       </c>
@@ -4292,7 +4513,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="98" spans="1:7" ht="12.95" thickBot="1">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A98" s="3" t="s">
         <v>292</v>
       </c>
@@ -4315,7 +4536,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="99" spans="1:7" ht="12.95" thickBot="1">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A99" s="3" t="s">
         <v>294</v>
       </c>
@@ -4338,7 +4559,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="100" spans="1:7" ht="12.95" thickBot="1">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A100" s="3" t="s">
         <v>297</v>
       </c>
@@ -4361,7 +4582,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="101" spans="1:7" ht="12.95" thickBot="1">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A101" s="3" t="s">
         <v>300</v>
       </c>
@@ -4384,7 +4605,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="102" spans="1:7" ht="12.95" thickBot="1">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A102" s="3" t="s">
         <v>303</v>
       </c>
@@ -4407,7 +4628,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="103" spans="1:7" ht="12.95" thickBot="1">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A103" s="3" t="s">
         <v>305</v>
       </c>
@@ -4430,7 +4651,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="104" spans="1:7" ht="12.95" thickBot="1">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A104" s="3" t="s">
         <v>308</v>
       </c>
@@ -4453,7 +4674,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="105" spans="1:7" ht="12.95" thickBot="1">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A105" s="3" t="s">
         <v>311</v>
       </c>
@@ -4476,7 +4697,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="106" spans="1:7" ht="12.95" thickBot="1">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A106" s="3" t="s">
         <v>314</v>
       </c>
@@ -4499,7 +4720,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="107" spans="1:7" ht="12.95" thickBot="1">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A107" s="3" t="s">
         <v>317</v>
       </c>
@@ -4522,7 +4743,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="108" spans="1:7" ht="12.95" thickBot="1">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A108" s="3" t="s">
         <v>319</v>
       </c>
@@ -4545,7 +4766,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="109" spans="1:7" ht="12.95" thickBot="1">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A109" s="3" t="s">
         <v>322</v>
       </c>
@@ -4568,7 +4789,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="110" spans="1:7" ht="12.95" thickBot="1">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A110" s="3" t="s">
         <v>325</v>
       </c>
@@ -4591,7 +4812,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="111" spans="1:7" ht="12.95" thickBot="1">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A111" s="3" t="s">
         <v>328</v>
       </c>
@@ -4614,7 +4835,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="112" spans="1:7" ht="12.95" thickBot="1">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A112" s="3" t="s">
         <v>331</v>
       </c>
@@ -4637,7 +4858,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="113" spans="1:7" ht="12.95" thickBot="1">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A113" s="3" t="s">
         <v>334</v>
       </c>
@@ -4660,7 +4881,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="114" spans="1:7" ht="12.95" thickBot="1">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A114" s="3" t="s">
         <v>337</v>
       </c>
@@ -4683,7 +4904,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="115" spans="1:7" ht="12.95" thickBot="1">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A115" s="3" t="s">
         <v>339</v>
       </c>
@@ -4706,7 +4927,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="116" spans="1:7" ht="12.95" thickBot="1">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A116" s="3" t="s">
         <v>341</v>
       </c>
@@ -4729,7 +4950,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="117" spans="1:7" ht="12.95" thickBot="1">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A117" s="3" t="s">
         <v>344</v>
       </c>
@@ -4752,7 +4973,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="118" spans="1:7" ht="12.95" thickBot="1">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A118" s="3" t="s">
         <v>347</v>
       </c>
@@ -4775,7 +4996,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="119" spans="1:7" ht="12.95" thickBot="1">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A119" s="3" t="s">
         <v>350</v>
       </c>
@@ -4798,7 +5019,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="120" spans="1:7" ht="12.95" thickBot="1">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A120" s="3" t="s">
         <v>353</v>
       </c>
@@ -4821,7 +5042,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="121" spans="1:7" ht="12.95" thickBot="1">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A121" s="3" t="s">
         <v>356</v>
       </c>
@@ -4844,7 +5065,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="122" spans="1:7" ht="12.95" thickBot="1">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A122" s="3" t="s">
         <v>358</v>
       </c>
@@ -4867,7 +5088,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="123" spans="1:7" ht="12.95" thickBot="1">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A123" s="3" t="s">
         <v>361</v>
       </c>
@@ -4890,7 +5111,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="124" spans="1:7" ht="12.95" thickBot="1">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A124" s="3" t="s">
         <v>364</v>
       </c>
@@ -4913,7 +5134,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="125" spans="1:7" ht="12.95" thickBot="1">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A125" s="3" t="s">
         <v>366</v>
       </c>
@@ -4936,7 +5157,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="126" spans="1:7" ht="12.95" thickBot="1">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A126" s="3" t="s">
         <v>369</v>
       </c>
@@ -4959,7 +5180,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="127" spans="1:7" ht="12.95" thickBot="1">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A127" s="3" t="s">
         <v>371</v>
       </c>
@@ -4982,7 +5203,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="128" spans="1:7" ht="12.95" thickBot="1">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A128" s="3" t="s">
         <v>374</v>
       </c>
@@ -5005,7 +5226,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="129" spans="1:7" ht="12.95" thickBot="1">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A129" s="3" t="s">
         <v>376</v>
       </c>
@@ -5028,7 +5249,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="130" spans="1:7" ht="12.95" thickBot="1">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A130" s="3" t="s">
         <v>378</v>
       </c>
@@ -5051,7 +5272,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="131" spans="1:7" ht="12.95" thickBot="1">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A131" s="3" t="s">
         <v>381</v>
       </c>
@@ -5074,7 +5295,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="132" spans="1:7" ht="12.95" thickBot="1">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A132" s="3" t="s">
         <v>384</v>
       </c>
@@ -5097,7 +5318,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="133" spans="1:7" ht="12.95" thickBot="1">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A133" s="3" t="s">
         <v>387</v>
       </c>
@@ -5120,7 +5341,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="134" spans="1:7" ht="12.95" thickBot="1">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A134" s="3" t="s">
         <v>390</v>
       </c>
@@ -5143,7 +5364,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="135" spans="1:7" ht="12.95" thickBot="1">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A135" s="3" t="s">
         <v>392</v>
       </c>
@@ -5166,7 +5387,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="136" spans="1:7" ht="12.95" thickBot="1">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A136" s="3" t="s">
         <v>395</v>
       </c>
@@ -5189,7 +5410,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="137" spans="1:7" ht="12.95" thickBot="1">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A137" s="3" t="s">
         <v>397</v>
       </c>
@@ -5212,7 +5433,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="138" spans="1:7" ht="12.95" thickBot="1">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A138" s="3" t="s">
         <v>400</v>
       </c>
@@ -5235,7 +5456,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="139" spans="1:7" ht="12.95" thickBot="1">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A139" s="3" t="s">
         <v>403</v>
       </c>
@@ -5258,7 +5479,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="140" spans="1:7" ht="12.95" thickBot="1">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A140" s="3" t="s">
         <v>406</v>
       </c>
@@ -5281,7 +5502,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="141" spans="1:7" ht="12.95" thickBot="1">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A141" s="3" t="s">
         <v>409</v>
       </c>
@@ -5304,7 +5525,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="142" spans="1:7" ht="12.95" thickBot="1">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A142" s="3" t="s">
         <v>411</v>
       </c>
@@ -5327,7 +5548,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="143" spans="1:7" ht="12.95" thickBot="1">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A143" s="3" t="s">
         <v>414</v>
       </c>
@@ -5350,7 +5571,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="144" spans="1:7" ht="12.95" thickBot="1">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A144" s="3" t="s">
         <v>415</v>
       </c>
@@ -5373,7 +5594,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="145" spans="1:7" ht="12.95" thickBot="1">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A145" s="3" t="s">
         <v>418</v>
       </c>
@@ -5396,7 +5617,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="146" spans="1:7" ht="12.95" thickBot="1">
+    <row r="146" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A146" s="3" t="s">
         <v>421</v>
       </c>
@@ -5419,7 +5640,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="147" spans="1:7" ht="12.95" thickBot="1">
+    <row r="147" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A147" s="3" t="s">
         <v>424</v>
       </c>
@@ -5442,7 +5663,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="148" spans="1:7" ht="12.95" thickBot="1">
+    <row r="148" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A148" s="3" t="s">
         <v>427</v>
       </c>
@@ -5465,7 +5686,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="149" spans="1:7" ht="12.95" thickBot="1">
+    <row r="149" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A149" s="3" t="s">
         <v>429</v>
       </c>
@@ -5488,7 +5709,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="150" spans="1:7" ht="12.95" thickBot="1">
+    <row r="150" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A150" s="3" t="s">
         <v>432</v>
       </c>
@@ -5511,7 +5732,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="151" spans="1:7" ht="12.95" thickBot="1">
+    <row r="151" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A151" s="3" t="s">
         <v>434</v>
       </c>
@@ -5534,7 +5755,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="152" spans="1:7" ht="12.95" thickBot="1">
+    <row r="152" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A152" s="3" t="s">
         <v>437</v>
       </c>
@@ -5557,7 +5778,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="153" spans="1:7" ht="12.95" thickBot="1">
+    <row r="153" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A153" s="3" t="s">
         <v>440</v>
       </c>
@@ -5580,7 +5801,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="154" spans="1:7" ht="12.95" thickBot="1">
+    <row r="154" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A154" s="3" t="s">
         <v>442</v>
       </c>
@@ -5603,7 +5824,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="155" spans="1:7" ht="12.95" thickBot="1">
+    <row r="155" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A155" s="3" t="s">
         <v>444</v>
       </c>
@@ -5626,7 +5847,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="156" spans="1:7" ht="12.95" thickBot="1">
+    <row r="156" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A156" s="3" t="s">
         <v>447</v>
       </c>
@@ -5649,7 +5870,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="157" spans="1:7" ht="12.95" thickBot="1">
+    <row r="157" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A157" s="3" t="s">
         <v>450</v>
       </c>
@@ -5672,7 +5893,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="158" spans="1:7" ht="12.95" thickBot="1">
+    <row r="158" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A158" s="3" t="s">
         <v>453</v>
       </c>
@@ -5695,7 +5916,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="159" spans="1:7" ht="12.95" thickBot="1">
+    <row r="159" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A159" s="3" t="s">
         <v>456</v>
       </c>
@@ -5718,7 +5939,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="160" spans="1:7" ht="12.95" thickBot="1">
+    <row r="160" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A160" s="3" t="s">
         <v>459</v>
       </c>
@@ -5741,7 +5962,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="161" spans="1:7" ht="12.95" thickBot="1">
+    <row r="161" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A161" s="3" t="s">
         <v>462</v>
       </c>
@@ -5764,7 +5985,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="162" spans="1:7" ht="12.95" thickBot="1">
+    <row r="162" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A162" s="3" t="s">
         <v>465</v>
       </c>
@@ -5787,7 +6008,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="163" spans="1:7" ht="12.95" thickBot="1">
+    <row r="163" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A163" s="3" t="s">
         <v>467</v>
       </c>
@@ -5810,7 +6031,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="164" spans="1:7" ht="12.95" thickBot="1">
+    <row r="164" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A164" s="3" t="s">
         <v>470</v>
       </c>
@@ -5833,7 +6054,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="165" spans="1:7" ht="12.95" thickBot="1">
+    <row r="165" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A165" s="3" t="s">
         <v>473</v>
       </c>
@@ -5856,7 +6077,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="166" spans="1:7" ht="12.95" thickBot="1">
+    <row r="166" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A166" s="3" t="s">
         <v>475</v>
       </c>
@@ -5879,7 +6100,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="167" spans="1:7" ht="12.95" thickBot="1">
+    <row r="167" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A167" s="3" t="s">
         <v>478</v>
       </c>
@@ -5902,7 +6123,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="168" spans="1:7" ht="12.95" thickBot="1">
+    <row r="168" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A168" s="3" t="s">
         <v>481</v>
       </c>
@@ -5925,7 +6146,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="169" spans="1:7" ht="12.95" thickBot="1">
+    <row r="169" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A169" s="3" t="s">
         <v>483</v>
       </c>
@@ -5948,7 +6169,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="170" spans="1:7" ht="12.95" thickBot="1">
+    <row r="170" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A170" s="3" t="s">
         <v>486</v>
       </c>
@@ -5971,7 +6192,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="171" spans="1:7" ht="12.95" thickBot="1">
+    <row r="171" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A171" s="3" t="s">
         <v>488</v>
       </c>
@@ -5994,7 +6215,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="172" spans="1:7" ht="12.95" thickBot="1">
+    <row r="172" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A172" s="3" t="s">
         <v>491</v>
       </c>
@@ -6017,7 +6238,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="173" spans="1:7" ht="12.95" thickBot="1">
+    <row r="173" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A173" s="3" t="s">
         <v>494</v>
       </c>
@@ -6040,7 +6261,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="174" spans="1:7" ht="12.95" thickBot="1">
+    <row r="174" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A174" s="3" t="s">
         <v>496</v>
       </c>
@@ -6063,7 +6284,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="175" spans="1:7" ht="12.95" thickBot="1">
+    <row r="175" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A175" s="3" t="s">
         <v>499</v>
       </c>
@@ -6086,7 +6307,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="176" spans="1:7" ht="12.95" thickBot="1">
+    <row r="176" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A176" s="3" t="s">
         <v>502</v>
       </c>
@@ -6109,7 +6330,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="177" spans="1:7" ht="12.95" thickBot="1">
+    <row r="177" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A177" s="3" t="s">
         <v>504</v>
       </c>
@@ -6132,7 +6353,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="178" spans="1:7" ht="12.95" thickBot="1">
+    <row r="178" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A178" s="3" t="s">
         <v>506</v>
       </c>
@@ -6155,7 +6376,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="179" spans="1:7" ht="12.95" thickBot="1">
+    <row r="179" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A179" s="3" t="s">
         <v>509</v>
       </c>
@@ -6178,7 +6399,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="180" spans="1:7" ht="12.95" thickBot="1">
+    <row r="180" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A180" s="3" t="s">
         <v>512</v>
       </c>
@@ -6201,7 +6422,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="181" spans="1:7" ht="12.95" thickBot="1">
+    <row r="181" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A181" s="3" t="s">
         <v>515</v>
       </c>
@@ -6224,7 +6445,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="182" spans="1:7" ht="12.95" thickBot="1">
+    <row r="182" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A182" s="3" t="s">
         <v>518</v>
       </c>
@@ -6247,7 +6468,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="183" spans="1:7" ht="12.95" thickBot="1">
+    <row r="183" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A183" s="3" t="s">
         <v>521</v>
       </c>
@@ -6270,7 +6491,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="184" spans="1:7" ht="12.95" thickBot="1">
+    <row r="184" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A184" s="3" t="s">
         <v>523</v>
       </c>
@@ -6293,7 +6514,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="185" spans="1:7" ht="12.95" thickBot="1">
+    <row r="185" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A185" s="3" t="s">
         <v>526</v>
       </c>
@@ -6314,6 +6535,1608 @@
       </c>
       <c r="G185" s="1" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="186" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A186" s="6">
+        <v>627199</v>
+      </c>
+      <c r="B186" s="6" t="s">
+        <v>530</v>
+      </c>
+      <c r="C186" s="6" t="s">
+        <v>529</v>
+      </c>
+      <c r="D186" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E186" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F186" s="6">
+        <v>2025</v>
+      </c>
+      <c r="G186" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="187" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A187" s="6">
+        <v>975150</v>
+      </c>
+      <c r="B187" s="6" t="s">
+        <v>531</v>
+      </c>
+      <c r="C187" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D187" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E187" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F187" s="6">
+        <v>2026</v>
+      </c>
+      <c r="G187" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="188" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A188" s="6">
+        <v>118990</v>
+      </c>
+      <c r="B188" s="6" t="s">
+        <v>533</v>
+      </c>
+      <c r="C188" s="6" t="s">
+        <v>532</v>
+      </c>
+      <c r="D188" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="E188" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F188" s="6">
+        <v>2026</v>
+      </c>
+      <c r="G188" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="189" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A189" s="6">
+        <v>118423</v>
+      </c>
+      <c r="B189" s="6" t="s">
+        <v>534</v>
+      </c>
+      <c r="C189" s="6" t="s">
+        <v>452</v>
+      </c>
+      <c r="D189" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E189" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F189" s="6">
+        <v>2024</v>
+      </c>
+      <c r="G189" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="190" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A190" s="6">
+        <v>118512</v>
+      </c>
+      <c r="B190" s="6" t="s">
+        <v>535</v>
+      </c>
+      <c r="C190" s="6" t="s">
+        <v>346</v>
+      </c>
+      <c r="D190" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E190" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F190" s="6">
+        <v>2025</v>
+      </c>
+      <c r="G190" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="191" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A191" s="6">
+        <v>118512</v>
+      </c>
+      <c r="B191" s="6" t="s">
+        <v>535</v>
+      </c>
+      <c r="C191" s="6" t="s">
+        <v>346</v>
+      </c>
+      <c r="D191" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E191" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F191" s="6">
+        <v>2025</v>
+      </c>
+      <c r="G191" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="192" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A192" s="6">
+        <v>118512</v>
+      </c>
+      <c r="B192" s="6" t="s">
+        <v>535</v>
+      </c>
+      <c r="C192" s="6" t="s">
+        <v>346</v>
+      </c>
+      <c r="D192" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E192" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F192" s="6">
+        <v>2025</v>
+      </c>
+      <c r="G192" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="193" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A193" s="6">
+        <v>118535</v>
+      </c>
+      <c r="B193" s="6" t="s">
+        <v>537</v>
+      </c>
+      <c r="C193" s="6" t="s">
+        <v>536</v>
+      </c>
+      <c r="D193" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E193" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F193" s="6">
+        <v>2025</v>
+      </c>
+      <c r="G193" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="194" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A194" s="6">
+        <v>118535</v>
+      </c>
+      <c r="B194" s="6" t="s">
+        <v>537</v>
+      </c>
+      <c r="C194" s="6" t="s">
+        <v>536</v>
+      </c>
+      <c r="D194" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E194" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F194" s="6">
+        <v>2025</v>
+      </c>
+      <c r="G194" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="195" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A195" s="6">
+        <v>118619</v>
+      </c>
+      <c r="B195" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="C195" s="6" t="s">
+        <v>538</v>
+      </c>
+      <c r="D195" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E195" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F195" s="6">
+        <v>2025</v>
+      </c>
+      <c r="G195" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="196" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A196" s="6">
+        <v>118633</v>
+      </c>
+      <c r="B196" s="6" t="s">
+        <v>540</v>
+      </c>
+      <c r="C196" s="6" t="s">
+        <v>539</v>
+      </c>
+      <c r="D196" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E196" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F196" s="6">
+        <v>2024</v>
+      </c>
+      <c r="G196" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="197" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A197" s="6">
+        <v>118680</v>
+      </c>
+      <c r="B197" s="6" t="s">
+        <v>542</v>
+      </c>
+      <c r="C197" s="6" t="s">
+        <v>541</v>
+      </c>
+      <c r="D197" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E197" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F197" s="6">
+        <v>2025</v>
+      </c>
+      <c r="G197" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="198" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A198" s="6">
+        <v>119074</v>
+      </c>
+      <c r="B198" s="6" t="s">
+        <v>544</v>
+      </c>
+      <c r="C198" s="6" t="s">
+        <v>543</v>
+      </c>
+      <c r="D198" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E198" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F198" s="6">
+        <v>2025</v>
+      </c>
+      <c r="G198" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="199" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A199" s="6">
+        <v>119297</v>
+      </c>
+      <c r="B199" s="6" t="s">
+        <v>546</v>
+      </c>
+      <c r="C199" s="6" t="s">
+        <v>545</v>
+      </c>
+      <c r="D199" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E199" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F199" s="6">
+        <v>2027</v>
+      </c>
+      <c r="G199" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="200" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A200" s="6">
+        <v>200343</v>
+      </c>
+      <c r="B200" s="6" t="s">
+        <v>547</v>
+      </c>
+      <c r="C200" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="D200" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E200" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F200" s="6">
+        <v>2025</v>
+      </c>
+      <c r="G200" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="201" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A201" s="6">
+        <v>700300</v>
+      </c>
+      <c r="B201" s="6" t="s">
+        <v>549</v>
+      </c>
+      <c r="C201" s="6" t="s">
+        <v>548</v>
+      </c>
+      <c r="D201" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E201" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F201" s="6">
+        <v>2025</v>
+      </c>
+      <c r="G201" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="202" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A202" s="6">
+        <v>705247</v>
+      </c>
+      <c r="B202" s="6" t="s">
+        <v>551</v>
+      </c>
+      <c r="C202" s="6" t="s">
+        <v>550</v>
+      </c>
+      <c r="D202" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E202" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F202" s="6">
+        <v>2026</v>
+      </c>
+      <c r="G202" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="203" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A203" s="6">
+        <v>709828</v>
+      </c>
+      <c r="B203" s="6" t="s">
+        <v>552</v>
+      </c>
+      <c r="C203" s="6" t="s">
+        <v>241</v>
+      </c>
+      <c r="D203" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="E203" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F203" s="6">
+        <v>2024</v>
+      </c>
+      <c r="G203" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="204" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A204" s="6">
+        <v>724901</v>
+      </c>
+      <c r="B204" s="6" t="s">
+        <v>554</v>
+      </c>
+      <c r="C204" s="6" t="s">
+        <v>553</v>
+      </c>
+      <c r="D204" s="6" t="s">
+        <v>555</v>
+      </c>
+      <c r="E204" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F204" s="6">
+        <v>2025</v>
+      </c>
+      <c r="G204" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="205" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A205" s="6">
+        <v>725469</v>
+      </c>
+      <c r="B205" s="6" t="s">
+        <v>534</v>
+      </c>
+      <c r="C205" s="6" t="s">
+        <v>556</v>
+      </c>
+      <c r="D205" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E205" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F205" s="6">
+        <v>2027</v>
+      </c>
+      <c r="G205" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="206" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A206" s="6">
+        <v>750251</v>
+      </c>
+      <c r="B206" s="6" t="s">
+        <v>558</v>
+      </c>
+      <c r="C206" s="6" t="s">
+        <v>557</v>
+      </c>
+      <c r="D206" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E206" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F206" s="6">
+        <v>2027</v>
+      </c>
+      <c r="G206" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="207" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A207" s="6">
+        <v>752164</v>
+      </c>
+      <c r="B207" s="6" t="s">
+        <v>560</v>
+      </c>
+      <c r="C207" s="6" t="s">
+        <v>559</v>
+      </c>
+      <c r="D207" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E207" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F207" s="6">
+        <v>2025</v>
+      </c>
+      <c r="G207" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="208" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A208" s="6">
+        <v>752164</v>
+      </c>
+      <c r="B208" s="6" t="s">
+        <v>560</v>
+      </c>
+      <c r="C208" s="6" t="s">
+        <v>559</v>
+      </c>
+      <c r="D208" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E208" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F208" s="6">
+        <v>2025</v>
+      </c>
+      <c r="G208" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="209" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A209" s="6">
+        <v>752164</v>
+      </c>
+      <c r="B209" s="6" t="s">
+        <v>560</v>
+      </c>
+      <c r="C209" s="6" t="s">
+        <v>559</v>
+      </c>
+      <c r="D209" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E209" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F209" s="6">
+        <v>2025</v>
+      </c>
+      <c r="G209" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="210" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A210" s="6">
+        <v>763331</v>
+      </c>
+      <c r="B210" s="6" t="s">
+        <v>562</v>
+      </c>
+      <c r="C210" s="6" t="s">
+        <v>561</v>
+      </c>
+      <c r="D210" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E210" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F210" s="6">
+        <v>2026</v>
+      </c>
+      <c r="G210" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="211" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A211" s="6">
+        <v>763331</v>
+      </c>
+      <c r="B211" s="6" t="s">
+        <v>562</v>
+      </c>
+      <c r="C211" s="6" t="s">
+        <v>561</v>
+      </c>
+      <c r="D211" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E211" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F211" s="6">
+        <v>2026</v>
+      </c>
+      <c r="G211" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="212" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A212" s="6">
+        <v>764963</v>
+      </c>
+      <c r="B212" s="6" t="s">
+        <v>564</v>
+      </c>
+      <c r="C212" s="6" t="s">
+        <v>563</v>
+      </c>
+      <c r="D212" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E212" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F212" s="6">
+        <v>2026</v>
+      </c>
+      <c r="G212" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="213" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A213" s="6">
+        <v>764963</v>
+      </c>
+      <c r="B213" s="6" t="s">
+        <v>564</v>
+      </c>
+      <c r="C213" s="6" t="s">
+        <v>563</v>
+      </c>
+      <c r="D213" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E213" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F213" s="6">
+        <v>2026</v>
+      </c>
+      <c r="G213" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="214" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A214" s="6">
+        <v>764963</v>
+      </c>
+      <c r="B214" s="6" t="s">
+        <v>564</v>
+      </c>
+      <c r="C214" s="6" t="s">
+        <v>563</v>
+      </c>
+      <c r="D214" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E214" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F214" s="6">
+        <v>2026</v>
+      </c>
+      <c r="G214" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="215" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A215" s="6">
+        <v>769657</v>
+      </c>
+      <c r="B215" s="6" t="s">
+        <v>566</v>
+      </c>
+      <c r="C215" s="6" t="s">
+        <v>565</v>
+      </c>
+      <c r="D215" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E215" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F215" s="6">
+        <v>2026</v>
+      </c>
+      <c r="G215" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="216" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A216" s="6">
+        <v>772915</v>
+      </c>
+      <c r="B216" s="6" t="s">
+        <v>567</v>
+      </c>
+      <c r="C216" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="D216" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E216" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F216" s="6">
+        <v>2027</v>
+      </c>
+      <c r="G216" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="217" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A217" s="6">
+        <v>784998</v>
+      </c>
+      <c r="B217" s="6" t="s">
+        <v>569</v>
+      </c>
+      <c r="C217" s="6" t="s">
+        <v>568</v>
+      </c>
+      <c r="D217" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E217" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F217" s="6">
+        <v>2026</v>
+      </c>
+      <c r="G217" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="218" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A218" s="6">
+        <v>784998</v>
+      </c>
+      <c r="B218" s="6" t="s">
+        <v>569</v>
+      </c>
+      <c r="C218" s="6" t="s">
+        <v>568</v>
+      </c>
+      <c r="D218" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E218" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F218" s="6">
+        <v>2026</v>
+      </c>
+      <c r="G218" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="219" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A219" s="6">
+        <v>817615</v>
+      </c>
+      <c r="B219" s="6" t="s">
+        <v>571</v>
+      </c>
+      <c r="C219" s="6" t="s">
+        <v>570</v>
+      </c>
+      <c r="D219" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E219" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F219" s="6">
+        <v>2026</v>
+      </c>
+      <c r="G219" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="220" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A220" s="6">
+        <v>822371</v>
+      </c>
+      <c r="B220" s="6" t="s">
+        <v>412</v>
+      </c>
+      <c r="C220" s="6" t="s">
+        <v>310</v>
+      </c>
+      <c r="D220" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="E220" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F220" s="6">
+        <v>2027</v>
+      </c>
+      <c r="G220" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="221" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A221" s="6">
+        <v>822371</v>
+      </c>
+      <c r="B221" s="6" t="s">
+        <v>412</v>
+      </c>
+      <c r="C221" s="6" t="s">
+        <v>310</v>
+      </c>
+      <c r="D221" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="E221" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F221" s="6">
+        <v>2027</v>
+      </c>
+      <c r="G221" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="222" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A222" s="6">
+        <v>826295</v>
+      </c>
+      <c r="B222" s="6" t="s">
+        <v>573</v>
+      </c>
+      <c r="C222" s="6" t="s">
+        <v>572</v>
+      </c>
+      <c r="D222" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E222" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F222" s="6">
+        <v>2027</v>
+      </c>
+      <c r="G222" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="223" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A223" s="6">
+        <v>840189</v>
+      </c>
+      <c r="B223" s="6" t="s">
+        <v>575</v>
+      </c>
+      <c r="C223" s="6" t="s">
+        <v>574</v>
+      </c>
+      <c r="D223" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E223" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F223" s="6">
+        <v>2025</v>
+      </c>
+      <c r="G223" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="224" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A224" s="6">
+        <v>848012</v>
+      </c>
+      <c r="B224" s="6" t="s">
+        <v>576</v>
+      </c>
+      <c r="C224" s="6" t="s">
+        <v>550</v>
+      </c>
+      <c r="D224" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E224" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F224" s="6">
+        <v>2027</v>
+      </c>
+      <c r="G224" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="225" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A225" s="6">
+        <v>848012</v>
+      </c>
+      <c r="B225" s="6" t="s">
+        <v>576</v>
+      </c>
+      <c r="C225" s="6" t="s">
+        <v>550</v>
+      </c>
+      <c r="D225" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E225" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F225" s="6">
+        <v>2027</v>
+      </c>
+      <c r="G225" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="226" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A226" s="6">
+        <v>848012</v>
+      </c>
+      <c r="B226" s="6" t="s">
+        <v>576</v>
+      </c>
+      <c r="C226" s="6" t="s">
+        <v>550</v>
+      </c>
+      <c r="D226" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E226" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F226" s="6">
+        <v>2027</v>
+      </c>
+      <c r="G226" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="227" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A227" s="6">
+        <v>848012</v>
+      </c>
+      <c r="B227" s="6" t="s">
+        <v>576</v>
+      </c>
+      <c r="C227" s="6" t="s">
+        <v>550</v>
+      </c>
+      <c r="D227" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E227" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F227" s="6">
+        <v>2027</v>
+      </c>
+      <c r="G227" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="228" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A228" s="6">
+        <v>848075</v>
+      </c>
+      <c r="B228" s="6" t="s">
+        <v>578</v>
+      </c>
+      <c r="C228" s="6" t="s">
+        <v>577</v>
+      </c>
+      <c r="D228" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E228" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F228" s="6">
+        <v>2027</v>
+      </c>
+      <c r="G228" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="229" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A229" s="6">
+        <v>848075</v>
+      </c>
+      <c r="B229" s="6" t="s">
+        <v>578</v>
+      </c>
+      <c r="C229" s="6" t="s">
+        <v>577</v>
+      </c>
+      <c r="D229" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E229" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F229" s="6">
+        <v>2027</v>
+      </c>
+      <c r="G229" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="230" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A230" s="6">
+        <v>853875</v>
+      </c>
+      <c r="B230" s="6" t="s">
+        <v>580</v>
+      </c>
+      <c r="C230" s="6" t="s">
+        <v>579</v>
+      </c>
+      <c r="D230" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E230" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F230" s="6">
+        <v>2025</v>
+      </c>
+      <c r="G230" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="231" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A231" s="6">
+        <v>865008</v>
+      </c>
+      <c r="B231" s="6" t="s">
+        <v>581</v>
+      </c>
+      <c r="C231" s="6" t="s">
+        <v>452</v>
+      </c>
+      <c r="D231" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E231" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F231" s="6">
+        <v>2027</v>
+      </c>
+      <c r="G231" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="232" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A232" s="6">
+        <v>869238</v>
+      </c>
+      <c r="B232" s="6" t="s">
+        <v>582</v>
+      </c>
+      <c r="C232" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="D232" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E232" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F232" s="6">
+        <v>2026</v>
+      </c>
+      <c r="G232" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="233" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A233" s="6">
+        <v>869238</v>
+      </c>
+      <c r="B233" s="6" t="s">
+        <v>582</v>
+      </c>
+      <c r="C233" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="D233" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E233" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F233" s="6">
+        <v>2026</v>
+      </c>
+      <c r="G233" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="234" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A234" s="6">
+        <v>877560</v>
+      </c>
+      <c r="B234" s="6" t="s">
+        <v>584</v>
+      </c>
+      <c r="C234" s="6" t="s">
+        <v>583</v>
+      </c>
+      <c r="D234" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E234" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F234" s="6">
+        <v>2027</v>
+      </c>
+      <c r="G234" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="235" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A235" s="6">
+        <v>902833</v>
+      </c>
+      <c r="B235" s="6" t="s">
+        <v>585</v>
+      </c>
+      <c r="C235" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D235" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="E235" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F235" s="6">
+        <v>2027</v>
+      </c>
+      <c r="G235" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="236" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A236" s="6">
+        <v>914725</v>
+      </c>
+      <c r="B236" s="6" t="s">
+        <v>587</v>
+      </c>
+      <c r="C236" s="6" t="s">
+        <v>586</v>
+      </c>
+      <c r="D236" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E236" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F236" s="6">
+        <v>2026</v>
+      </c>
+      <c r="G236" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="237" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A237" s="6">
+        <v>921923</v>
+      </c>
+      <c r="B237" s="6" t="s">
+        <v>589</v>
+      </c>
+      <c r="C237" s="6" t="s">
+        <v>588</v>
+      </c>
+      <c r="D237" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E237" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F237" s="6">
+        <v>2024</v>
+      </c>
+      <c r="G237" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="238" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A238" s="6">
+        <v>930935</v>
+      </c>
+      <c r="B238" s="6" t="s">
+        <v>591</v>
+      </c>
+      <c r="C238" s="6" t="s">
+        <v>590</v>
+      </c>
+      <c r="D238" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E238" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F238" s="6">
+        <v>2026</v>
+      </c>
+      <c r="G238" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="239" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A239" s="6">
+        <v>946622</v>
+      </c>
+      <c r="B239" s="6" t="s">
+        <v>593</v>
+      </c>
+      <c r="C239" s="6" t="s">
+        <v>592</v>
+      </c>
+      <c r="D239" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E239" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F239" s="6">
+        <v>2026</v>
+      </c>
+      <c r="G239" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="240" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A240" s="6">
+        <v>946622</v>
+      </c>
+      <c r="B240" s="6" t="s">
+        <v>593</v>
+      </c>
+      <c r="C240" s="6" t="s">
+        <v>592</v>
+      </c>
+      <c r="D240" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E240" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F240" s="6">
+        <v>2026</v>
+      </c>
+      <c r="G240" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="241" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A241" s="6">
+        <v>967159</v>
+      </c>
+      <c r="B241" s="6" t="s">
+        <v>595</v>
+      </c>
+      <c r="C241" s="6" t="s">
+        <v>594</v>
+      </c>
+      <c r="D241" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E241" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F241" s="6">
+        <v>2026</v>
+      </c>
+      <c r="G241" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="242" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A242" s="6">
+        <v>967159</v>
+      </c>
+      <c r="B242" s="6" t="s">
+        <v>595</v>
+      </c>
+      <c r="C242" s="6" t="s">
+        <v>594</v>
+      </c>
+      <c r="D242" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E242" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F242" s="6">
+        <v>2026</v>
+      </c>
+      <c r="G242" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="243" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A243" s="6">
+        <v>967159</v>
+      </c>
+      <c r="B243" s="6" t="s">
+        <v>595</v>
+      </c>
+      <c r="C243" s="6" t="s">
+        <v>594</v>
+      </c>
+      <c r="D243" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E243" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F243" s="6">
+        <v>2026</v>
+      </c>
+      <c r="G243" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="244" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A244" s="6">
+        <v>978318</v>
+      </c>
+      <c r="B244" s="6" t="s">
+        <v>596</v>
+      </c>
+      <c r="C244" s="6" t="s">
+        <v>313</v>
+      </c>
+      <c r="D244" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E244" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F244" s="6">
+        <v>2027</v>
+      </c>
+      <c r="G244" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="245" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A245" s="6">
+        <v>978318</v>
+      </c>
+      <c r="B245" s="6" t="s">
+        <v>596</v>
+      </c>
+      <c r="C245" s="6" t="s">
+        <v>313</v>
+      </c>
+      <c r="D245" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E245" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F245" s="6">
+        <v>2027</v>
+      </c>
+    </row>
+    <row r="246" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A246" s="6">
+        <v>978318</v>
+      </c>
+      <c r="B246" s="6" t="s">
+        <v>596</v>
+      </c>
+      <c r="C246" s="6" t="s">
+        <v>313</v>
+      </c>
+      <c r="D246" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E246" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F246" s="6">
+        <v>2027</v>
+      </c>
+    </row>
+    <row r="247" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A247" s="6">
+        <v>978318</v>
+      </c>
+      <c r="B247" s="6" t="s">
+        <v>596</v>
+      </c>
+      <c r="C247" s="6" t="s">
+        <v>313</v>
+      </c>
+      <c r="D247" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E247" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F247" s="6">
+        <v>2027</v>
+      </c>
+    </row>
+    <row r="248" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A248" s="6">
+        <v>978318</v>
+      </c>
+      <c r="B248" s="6" t="s">
+        <v>596</v>
+      </c>
+      <c r="C248" s="6" t="s">
+        <v>313</v>
+      </c>
+      <c r="D248" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E248" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F248" s="6">
+        <v>2027</v>
+      </c>
+    </row>
+    <row r="249" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A249" s="6">
+        <v>996050</v>
+      </c>
+      <c r="B249" s="6" t="s">
+        <v>597</v>
+      </c>
+      <c r="C249" s="6" t="s">
+        <v>501</v>
+      </c>
+      <c r="D249" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E249" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F249" s="6">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="250" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A250" s="6">
+        <v>996160</v>
+      </c>
+      <c r="B250" s="6" t="s">
+        <v>598</v>
+      </c>
+      <c r="C250" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="D250" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E250" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F250" s="6">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="251" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A251" s="6">
+        <v>999274</v>
+      </c>
+      <c r="B251" s="6" t="s">
+        <v>599</v>
+      </c>
+      <c r="C251" s="6" t="s">
+        <v>431</v>
+      </c>
+      <c r="D251" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E251" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F251" s="6">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="252" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A252" s="6">
+        <v>999274</v>
+      </c>
+      <c r="B252" s="6" t="s">
+        <v>599</v>
+      </c>
+      <c r="C252" s="6" t="s">
+        <v>431</v>
+      </c>
+      <c r="D252" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E252" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F252" s="6">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="253" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A253" s="6">
+        <v>999607</v>
+      </c>
+      <c r="B253" s="6" t="s">
+        <v>448</v>
+      </c>
+      <c r="C253" s="6" t="s">
+        <v>600</v>
+      </c>
+      <c r="D253" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E253" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F253" s="6">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="254" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A254" s="6">
+        <v>999712</v>
+      </c>
+      <c r="B254" s="6" t="s">
+        <v>602</v>
+      </c>
+      <c r="C254" s="6" t="s">
+        <v>601</v>
+      </c>
+      <c r="D254" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E254" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F254" s="6">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="255" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A255" s="6">
+        <v>999712</v>
+      </c>
+      <c r="B255" s="6" t="s">
+        <v>602</v>
+      </c>
+      <c r="C255" s="6" t="s">
+        <v>601</v>
+      </c>
+      <c r="D255" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E255" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F255" s="6">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="256" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A256" s="6">
+        <v>999712</v>
+      </c>
+      <c r="B256" s="6" t="s">
+        <v>602</v>
+      </c>
+      <c r="C256" s="6" t="s">
+        <v>601</v>
+      </c>
+      <c r="D256" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E256" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F256" s="6">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="257" spans="5:5" x14ac:dyDescent="0.15">
+      <c r="E257" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -6322,6 +8145,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="efce84db-8738-4c7b-9bdc-65b9500871f6" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="e4ac40dc-80da-4869-807e-191aa97932d8">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100150EF88E6C4F8C4F84FC71A82B3C6822" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="697e8debfdb234a79869f6601575b6d6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e4ac40dc-80da-4869-807e-191aa97932d8" xmlns:ns3="c8e8eaa7-2320-4408-9564-9ed5178ae212" xmlns:ns4="efce84db-8738-4c7b-9bdc-65b9500871f6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5c9d69cf304cf964841c7670fa87e56f" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="e4ac40dc-80da-4869-807e-191aa97932d8"/>
@@ -6567,34 +8410,41 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="efce84db-8738-4c7b-9bdc-65b9500871f6" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="e4ac40dc-80da-4869-807e-191aa97932d8">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{506B5D65-D17D-4B19-A762-8B542DECFC4D}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A5E07700-420E-46F7-9DE6-7AF35B4B035E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="efce84db-8738-4c7b-9bdc-65b9500871f6"/>
+    <ds:schemaRef ds:uri="e4ac40dc-80da-4869-807e-191aa97932d8"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A5E07700-420E-46F7-9DE6-7AF35B4B035E}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C1B82C93-0C8A-42A6-94D3-03BD21DA2B68}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C1B82C93-0C8A-42A6-94D3-03BD21DA2B68}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{506B5D65-D17D-4B19-A762-8B542DECFC4D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="e4ac40dc-80da-4869-807e-191aa97932d8"/>
+    <ds:schemaRef ds:uri="c8e8eaa7-2320-4408-9564-9ed5178ae212"/>
+    <ds:schemaRef ds:uri="efce84db-8738-4c7b-9bdc-65b9500871f6"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
updated demographic data, no students missing, updated attendance and exit slip data, copied over WiENG attendence report
</commit_message>
<xml_diff>
--- a/data/raw/student_dem_raw.xlsx
+++ b/data/raw/student_dem_raw.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28020"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sylviaboguniecki/Desktop/wistem_23_24/data/raw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\LIZ\WiSTEM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{256D63D9-FA55-EC4A-AF0B-17AE8D78029D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C1588637-C370-495B-A557-C010C4823F2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="19420" windowHeight="16720" xr2:uid="{C7C2B227-BBDA-4416-93C7-10628C12C90F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{C7C2B227-BBDA-4416-93C7-10628C12C90F}"/>
   </bookViews>
   <sheets>
     <sheet name="wistem" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1455" uniqueCount="603">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1481" uniqueCount="605">
   <si>
     <t>ID</t>
   </si>
@@ -1625,207 +1625,207 @@
     <t>Larkin</t>
   </si>
   <si>
+    <t>Shah</t>
+  </si>
+  <si>
     <t>Izzah</t>
   </si>
   <si>
-    <t>Shah</t>
-  </si>
-  <si>
     <t>Frajman</t>
   </si>
   <si>
+    <t>Peters</t>
+  </si>
+  <si>
     <t>Shaili</t>
   </si>
   <si>
-    <t>Peters</t>
-  </si>
-  <si>
     <t>Buell</t>
   </si>
   <si>
     <t>Freeman</t>
   </si>
   <si>
+    <t>Mordka</t>
+  </si>
+  <si>
     <t>Rivka</t>
   </si>
   <si>
-    <t>Mordka</t>
-  </si>
-  <si>
     <t>Natalya</t>
   </si>
   <si>
+    <t>Rodriguez</t>
+  </si>
+  <si>
     <t>Kayla</t>
   </si>
   <si>
-    <t>Rodriguez</t>
+    <t>Olko</t>
   </si>
   <si>
     <t>Ingrid</t>
   </si>
   <si>
-    <t>Olko</t>
+    <t>Kegler</t>
   </si>
   <si>
     <t>Sophie</t>
   </si>
   <si>
-    <t>Kegler</t>
+    <t>Villaruel</t>
   </si>
   <si>
     <t>Luenonie Ruvikk</t>
   </si>
   <si>
-    <t>Villaruel</t>
-  </si>
-  <si>
     <t>Gallo</t>
   </si>
   <si>
+    <t>Feeney</t>
+  </si>
+  <si>
     <t>Eleanor</t>
   </si>
   <si>
-    <t>Feeney</t>
+    <t>Mcdermott</t>
   </si>
   <si>
     <t>Casey</t>
   </si>
   <si>
-    <t>Mcdermott</t>
-  </si>
-  <si>
     <t>Lindsey</t>
   </si>
   <si>
+    <t>Corbett</t>
+  </si>
+  <si>
     <t>Cameron</t>
   </si>
   <si>
-    <t>Corbett</t>
-  </si>
-  <si>
     <t>American Indian or Alaska Native</t>
   </si>
   <si>
     <t>Clara</t>
   </si>
   <si>
+    <t>Hausman</t>
+  </si>
+  <si>
     <t>Makeda</t>
   </si>
   <si>
-    <t>Hausman</t>
+    <t>Amromin</t>
   </si>
   <si>
     <t>Leah</t>
   </si>
   <si>
-    <t>Amromin</t>
+    <t>Wade</t>
   </si>
   <si>
     <t>Frances</t>
   </si>
   <si>
-    <t>Wade</t>
+    <t>Frolichstein</t>
   </si>
   <si>
     <t>Jessica</t>
   </si>
   <si>
-    <t>Frolichstein</t>
+    <t>Waldron</t>
   </si>
   <si>
     <t>Oaklyn</t>
   </si>
   <si>
-    <t>Waldron</t>
-  </si>
-  <si>
     <t>Solar</t>
   </si>
   <si>
+    <t>Lagunilla</t>
+  </si>
+  <si>
     <t>Alondra</t>
   </si>
   <si>
-    <t>Lagunilla</t>
+    <t>Hogan</t>
   </si>
   <si>
     <t>Eliza</t>
   </si>
   <si>
-    <t>Hogan</t>
+    <t>Gojakovic</t>
   </si>
   <si>
     <t>Vanya</t>
   </si>
   <si>
-    <t>Gojakovic</t>
+    <t>Stringer</t>
   </si>
   <si>
     <t>Amiah</t>
   </si>
   <si>
-    <t>Stringer</t>
-  </si>
-  <si>
     <t>Martin</t>
   </si>
   <si>
+    <t>Keller</t>
+  </si>
+  <si>
     <t>Susannah</t>
   </si>
   <si>
-    <t>Keller</t>
+    <t>Cohn</t>
   </si>
   <si>
     <t>Penelope</t>
   </si>
   <si>
-    <t>Cohn</t>
-  </si>
-  <si>
     <t>Quail</t>
   </si>
   <si>
     <t>Harris</t>
   </si>
   <si>
+    <t>Solomon</t>
+  </si>
+  <si>
     <t>Vivian</t>
   </si>
   <si>
-    <t>Solomon</t>
-  </si>
-  <si>
     <t>Decastro</t>
   </si>
   <si>
+    <t>Vazquez</t>
+  </si>
+  <si>
     <t>Laissa</t>
   </si>
   <si>
-    <t>Vazquez</t>
+    <t>Acosta</t>
   </si>
   <si>
     <t>Natalia</t>
   </si>
   <si>
-    <t>Acosta</t>
+    <t>Kasprzycki</t>
   </si>
   <si>
     <t>Kelen</t>
   </si>
   <si>
-    <t>Kasprzycki</t>
+    <t>Kimrey</t>
   </si>
   <si>
     <t>Phoebe</t>
   </si>
   <si>
-    <t>Kimrey</t>
+    <t>Vera</t>
   </si>
   <si>
     <t>Naiyeli</t>
   </si>
   <si>
-    <t>Vera</t>
-  </si>
-  <si>
     <t>Weinert</t>
   </si>
   <si>
@@ -1841,10 +1841,16 @@
     <t>Thalia</t>
   </si>
   <si>
+    <t>O'Hare</t>
+  </si>
+  <si>
     <t>Molly</t>
   </si>
   <si>
-    <t>O'Hare</t>
+    <t>Scrimenti</t>
+  </si>
+  <si>
+    <t>Lucia</t>
   </si>
 </sst>
 </file>
@@ -1854,7 +1860,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -2271,18 +2277,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03138AD1-97AD-4498-9D2F-72B0C051055A}">
-  <dimension ref="A1:G257"/>
+  <dimension ref="A1:G259"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A229" workbookViewId="0">
-      <selection activeCell="M185" sqref="M185"/>
+    <sheetView tabSelected="1" topLeftCell="A222" workbookViewId="0">
+      <selection activeCell="F254" sqref="F254"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.19921875" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="10.5"/>
   <cols>
-    <col min="1" max="16384" width="9.19921875" style="6"/>
+    <col min="1" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" s="5" customFormat="1">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2305,7 +2311,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
@@ -2328,7 +2334,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7">
       <c r="A3" s="3" t="s">
         <v>13</v>
       </c>
@@ -2351,7 +2357,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7">
       <c r="A4" s="3" t="s">
         <v>17</v>
       </c>
@@ -2374,7 +2380,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7">
       <c r="A5" s="3" t="s">
         <v>19</v>
       </c>
@@ -2397,7 +2403,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7">
       <c r="A6" s="3" t="s">
         <v>22</v>
       </c>
@@ -2420,7 +2426,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7">
       <c r="A7" s="3" t="s">
         <v>26</v>
       </c>
@@ -2443,7 +2449,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7">
       <c r="A8" s="3" t="s">
         <v>30</v>
       </c>
@@ -2466,7 +2472,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7">
       <c r="A9" s="3" t="s">
         <v>33</v>
       </c>
@@ -2489,7 +2495,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7">
       <c r="A10" s="3" t="s">
         <v>36</v>
       </c>
@@ -2512,7 +2518,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7">
       <c r="A11" s="3" t="s">
         <v>39</v>
       </c>
@@ -2535,7 +2541,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7">
       <c r="A12" s="3" t="s">
         <v>42</v>
       </c>
@@ -2558,7 +2564,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:7">
       <c r="A13" s="3" t="s">
         <v>45</v>
       </c>
@@ -2581,7 +2587,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7">
       <c r="A14" s="3" t="s">
         <v>48</v>
       </c>
@@ -2604,7 +2610,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7">
       <c r="A15" s="3" t="s">
         <v>51</v>
       </c>
@@ -2627,7 +2633,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7">
       <c r="A16" s="3" t="s">
         <v>54</v>
       </c>
@@ -2650,7 +2656,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:7">
       <c r="A17" s="3" t="s">
         <v>57</v>
       </c>
@@ -2673,7 +2679,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:7">
       <c r="A18" s="3" t="s">
         <v>60</v>
       </c>
@@ -2696,7 +2702,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:7">
       <c r="A19" s="3" t="s">
         <v>63</v>
       </c>
@@ -2719,7 +2725,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:7">
       <c r="A20" s="3" t="s">
         <v>66</v>
       </c>
@@ -2742,7 +2748,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:7">
       <c r="A21" s="3" t="s">
         <v>69</v>
       </c>
@@ -2765,7 +2771,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:7">
       <c r="A22" s="3" t="s">
         <v>73</v>
       </c>
@@ -2788,7 +2794,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:7">
       <c r="A23" s="3" t="s">
         <v>76</v>
       </c>
@@ -2811,7 +2817,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:7">
       <c r="A24" s="3" t="s">
         <v>79</v>
       </c>
@@ -2834,7 +2840,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:7">
       <c r="A25" s="3" t="s">
         <v>82</v>
       </c>
@@ -2857,7 +2863,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:7">
       <c r="A26" s="3" t="s">
         <v>85</v>
       </c>
@@ -2880,7 +2886,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:7">
       <c r="A27" s="3" t="s">
         <v>88</v>
       </c>
@@ -2903,7 +2909,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:7">
       <c r="A28" s="3" t="s">
         <v>90</v>
       </c>
@@ -2926,7 +2932,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:7">
       <c r="A29" s="3" t="s">
         <v>93</v>
       </c>
@@ -2949,7 +2955,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:7">
       <c r="A30" s="3" t="s">
         <v>96</v>
       </c>
@@ -2972,7 +2978,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:7">
       <c r="A31" s="3" t="s">
         <v>99</v>
       </c>
@@ -2995,7 +3001,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:7">
       <c r="A32" s="3" t="s">
         <v>101</v>
       </c>
@@ -3018,7 +3024,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:7">
       <c r="A33" s="3" t="s">
         <v>103</v>
       </c>
@@ -3041,7 +3047,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:7">
       <c r="A34" s="3" t="s">
         <v>106</v>
       </c>
@@ -3064,7 +3070,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:7">
       <c r="A35" s="3" t="s">
         <v>109</v>
       </c>
@@ -3087,7 +3093,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:7">
       <c r="A36" s="3" t="s">
         <v>111</v>
       </c>
@@ -3110,7 +3116,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:7">
       <c r="A37" s="3" t="s">
         <v>114</v>
       </c>
@@ -3133,7 +3139,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:7">
       <c r="A38" s="3" t="s">
         <v>117</v>
       </c>
@@ -3156,7 +3162,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:7">
       <c r="A39" s="3" t="s">
         <v>120</v>
       </c>
@@ -3179,7 +3185,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:7">
       <c r="A40" s="3" t="s">
         <v>123</v>
       </c>
@@ -3202,7 +3208,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:7">
       <c r="A41" s="3" t="s">
         <v>126</v>
       </c>
@@ -3225,7 +3231,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:7">
       <c r="A42" s="3" t="s">
         <v>129</v>
       </c>
@@ -3248,7 +3254,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:7">
       <c r="A43" s="3" t="s">
         <v>132</v>
       </c>
@@ -3271,7 +3277,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:7">
       <c r="A44" s="3" t="s">
         <v>135</v>
       </c>
@@ -3294,7 +3300,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:7">
       <c r="A45" s="3" t="s">
         <v>138</v>
       </c>
@@ -3317,7 +3323,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:7">
       <c r="A46" s="3" t="s">
         <v>140</v>
       </c>
@@ -3340,7 +3346,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:7">
       <c r="A47" s="3" t="s">
         <v>143</v>
       </c>
@@ -3363,7 +3369,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:7">
       <c r="A48" s="3" t="s">
         <v>146</v>
       </c>
@@ -3386,7 +3392,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:7">
       <c r="A49" s="3" t="s">
         <v>148</v>
       </c>
@@ -3409,7 +3415,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:7">
       <c r="A50" s="3" t="s">
         <v>151</v>
       </c>
@@ -3432,7 +3438,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:7">
       <c r="A51" s="3" t="s">
         <v>154</v>
       </c>
@@ -3455,7 +3461,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:7">
       <c r="A52" s="3" t="s">
         <v>157</v>
       </c>
@@ -3478,7 +3484,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:7">
       <c r="A53" s="3" t="s">
         <v>160</v>
       </c>
@@ -3501,7 +3507,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:7">
       <c r="A54" s="3" t="s">
         <v>163</v>
       </c>
@@ -3524,7 +3530,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:7">
       <c r="A55" s="3" t="s">
         <v>166</v>
       </c>
@@ -3547,7 +3553,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:7">
       <c r="A56" s="3" t="s">
         <v>169</v>
       </c>
@@ -3570,7 +3576,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:7">
       <c r="A57" s="3" t="s">
         <v>172</v>
       </c>
@@ -3593,7 +3599,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:7">
       <c r="A58" s="3" t="s">
         <v>175</v>
       </c>
@@ -3616,7 +3622,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:7">
       <c r="A59" s="3" t="s">
         <v>178</v>
       </c>
@@ -3639,7 +3645,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:7">
       <c r="A60" s="3" t="s">
         <v>181</v>
       </c>
@@ -3662,7 +3668,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:7">
       <c r="A61" s="3" t="s">
         <v>184</v>
       </c>
@@ -3685,7 +3691,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:7">
       <c r="A62" s="3" t="s">
         <v>187</v>
       </c>
@@ -3708,7 +3714,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:7">
       <c r="A63" s="3" t="s">
         <v>190</v>
       </c>
@@ -3731,7 +3737,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:7">
       <c r="A64" s="3" t="s">
         <v>193</v>
       </c>
@@ -3754,7 +3760,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:7">
       <c r="A65" s="3" t="s">
         <v>196</v>
       </c>
@@ -3777,7 +3783,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:7">
       <c r="A66" s="3" t="s">
         <v>199</v>
       </c>
@@ -3800,7 +3806,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:7">
       <c r="A67" s="3" t="s">
         <v>202</v>
       </c>
@@ -3823,7 +3829,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:7">
       <c r="A68" s="3" t="s">
         <v>205</v>
       </c>
@@ -3846,7 +3852,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:7">
       <c r="A69" s="3" t="s">
         <v>208</v>
       </c>
@@ -3869,7 +3875,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:7">
       <c r="A70" s="3" t="s">
         <v>211</v>
       </c>
@@ -3892,7 +3898,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:7">
       <c r="A71" s="3" t="s">
         <v>214</v>
       </c>
@@ -3915,7 +3921,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:7">
       <c r="A72" s="3" t="s">
         <v>217</v>
       </c>
@@ -3938,7 +3944,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:7">
       <c r="A73" s="3" t="s">
         <v>219</v>
       </c>
@@ -3961,7 +3967,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:7">
       <c r="A74" s="3" t="s">
         <v>222</v>
       </c>
@@ -3984,7 +3990,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:7">
       <c r="A75" s="3" t="s">
         <v>225</v>
       </c>
@@ -4007,7 +4013,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:7">
       <c r="A76" s="3" t="s">
         <v>227</v>
       </c>
@@ -4030,7 +4036,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:7">
       <c r="A77" s="3" t="s">
         <v>230</v>
       </c>
@@ -4053,7 +4059,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:7">
       <c r="A78" s="3" t="s">
         <v>233</v>
       </c>
@@ -4076,7 +4082,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:7">
       <c r="A79" s="3" t="s">
         <v>236</v>
       </c>
@@ -4099,7 +4105,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:7">
       <c r="A80" s="3" t="s">
         <v>239</v>
       </c>
@@ -4122,7 +4128,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:7">
       <c r="A81" s="3" t="s">
         <v>242</v>
       </c>
@@ -4145,7 +4151,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:7">
       <c r="A82" s="3" t="s">
         <v>245</v>
       </c>
@@ -4168,7 +4174,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="83" spans="1:7">
       <c r="A83" s="3" t="s">
         <v>248</v>
       </c>
@@ -4191,7 +4197,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="84" spans="1:7">
       <c r="A84" s="3" t="s">
         <v>251</v>
       </c>
@@ -4214,7 +4220,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="85" spans="1:7">
       <c r="A85" s="3" t="s">
         <v>254</v>
       </c>
@@ -4237,7 +4243,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="86" spans="1:7">
       <c r="A86" s="3" t="s">
         <v>257</v>
       </c>
@@ -4260,7 +4266,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="87" spans="1:7">
       <c r="A87" s="3" t="s">
         <v>260</v>
       </c>
@@ -4283,7 +4289,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="88" spans="1:7">
       <c r="A88" s="3" t="s">
         <v>263</v>
       </c>
@@ -4306,7 +4312,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="89" spans="1:7">
       <c r="A89" s="3" t="s">
         <v>265</v>
       </c>
@@ -4329,7 +4335,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="90" spans="1:7">
       <c r="A90" s="3" t="s">
         <v>268</v>
       </c>
@@ -4352,7 +4358,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:7">
       <c r="A91" s="3" t="s">
         <v>271</v>
       </c>
@@ -4375,7 +4381,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="92" spans="1:7">
       <c r="A92" s="3" t="s">
         <v>274</v>
       </c>
@@ -4398,7 +4404,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="93" spans="1:7">
       <c r="A93" s="3" t="s">
         <v>277</v>
       </c>
@@ -4421,7 +4427,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="94" spans="1:7">
       <c r="A94" s="3" t="s">
         <v>280</v>
       </c>
@@ -4444,7 +4450,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="95" spans="1:7">
       <c r="A95" s="3" t="s">
         <v>283</v>
       </c>
@@ -4467,7 +4473,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="96" spans="1:7">
       <c r="A96" s="3" t="s">
         <v>286</v>
       </c>
@@ -4490,7 +4496,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="97" spans="1:7">
       <c r="A97" s="3" t="s">
         <v>289</v>
       </c>
@@ -4513,7 +4519,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="98" spans="1:7">
       <c r="A98" s="3" t="s">
         <v>292</v>
       </c>
@@ -4536,7 +4542,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="99" spans="1:7">
       <c r="A99" s="3" t="s">
         <v>294</v>
       </c>
@@ -4559,7 +4565,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="100" spans="1:7">
       <c r="A100" s="3" t="s">
         <v>297</v>
       </c>
@@ -4582,7 +4588,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="101" spans="1:7">
       <c r="A101" s="3" t="s">
         <v>300</v>
       </c>
@@ -4605,7 +4611,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="102" spans="1:7">
       <c r="A102" s="3" t="s">
         <v>303</v>
       </c>
@@ -4628,7 +4634,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="103" spans="1:7">
       <c r="A103" s="3" t="s">
         <v>305</v>
       </c>
@@ -4651,7 +4657,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="104" spans="1:7">
       <c r="A104" s="3" t="s">
         <v>308</v>
       </c>
@@ -4674,7 +4680,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="105" spans="1:7">
       <c r="A105" s="3" t="s">
         <v>311</v>
       </c>
@@ -4697,7 +4703,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="106" spans="1:7">
       <c r="A106" s="3" t="s">
         <v>314</v>
       </c>
@@ -4720,7 +4726,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="107" spans="1:7">
       <c r="A107" s="3" t="s">
         <v>317</v>
       </c>
@@ -4743,7 +4749,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="108" spans="1:7">
       <c r="A108" s="3" t="s">
         <v>319</v>
       </c>
@@ -4766,7 +4772,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="109" spans="1:7">
       <c r="A109" s="3" t="s">
         <v>322</v>
       </c>
@@ -4789,7 +4795,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="110" spans="1:7">
       <c r="A110" s="3" t="s">
         <v>325</v>
       </c>
@@ -4812,7 +4818,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="111" spans="1:7">
       <c r="A111" s="3" t="s">
         <v>328</v>
       </c>
@@ -4835,7 +4841,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="112" spans="1:7">
       <c r="A112" s="3" t="s">
         <v>331</v>
       </c>
@@ -4858,7 +4864,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="113" spans="1:7">
       <c r="A113" s="3" t="s">
         <v>334</v>
       </c>
@@ -4881,7 +4887,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="114" spans="1:7">
       <c r="A114" s="3" t="s">
         <v>337</v>
       </c>
@@ -4904,7 +4910,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="115" spans="1:7">
       <c r="A115" s="3" t="s">
         <v>339</v>
       </c>
@@ -4927,7 +4933,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="116" spans="1:7">
       <c r="A116" s="3" t="s">
         <v>341</v>
       </c>
@@ -4950,7 +4956,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="117" spans="1:7">
       <c r="A117" s="3" t="s">
         <v>344</v>
       </c>
@@ -4973,7 +4979,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="118" spans="1:7">
       <c r="A118" s="3" t="s">
         <v>347</v>
       </c>
@@ -4996,7 +5002,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="119" spans="1:7">
       <c r="A119" s="3" t="s">
         <v>350</v>
       </c>
@@ -5019,7 +5025,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="120" spans="1:7">
       <c r="A120" s="3" t="s">
         <v>353</v>
       </c>
@@ -5042,7 +5048,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="121" spans="1:7">
       <c r="A121" s="3" t="s">
         <v>356</v>
       </c>
@@ -5065,7 +5071,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="122" spans="1:7">
       <c r="A122" s="3" t="s">
         <v>358</v>
       </c>
@@ -5088,7 +5094,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="123" spans="1:7">
       <c r="A123" s="3" t="s">
         <v>361</v>
       </c>
@@ -5111,7 +5117,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="124" spans="1:7">
       <c r="A124" s="3" t="s">
         <v>364</v>
       </c>
@@ -5134,7 +5140,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="125" spans="1:7">
       <c r="A125" s="3" t="s">
         <v>366</v>
       </c>
@@ -5157,7 +5163,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="126" spans="1:7">
       <c r="A126" s="3" t="s">
         <v>369</v>
       </c>
@@ -5180,7 +5186,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="127" spans="1:7">
       <c r="A127" s="3" t="s">
         <v>371</v>
       </c>
@@ -5203,7 +5209,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="128" spans="1:7">
       <c r="A128" s="3" t="s">
         <v>374</v>
       </c>
@@ -5226,7 +5232,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="129" spans="1:7">
       <c r="A129" s="3" t="s">
         <v>376</v>
       </c>
@@ -5249,7 +5255,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="130" spans="1:7">
       <c r="A130" s="3" t="s">
         <v>378</v>
       </c>
@@ -5272,7 +5278,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="131" spans="1:7">
       <c r="A131" s="3" t="s">
         <v>381</v>
       </c>
@@ -5295,7 +5301,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="132" spans="1:7">
       <c r="A132" s="3" t="s">
         <v>384</v>
       </c>
@@ -5318,7 +5324,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="133" spans="1:7">
       <c r="A133" s="3" t="s">
         <v>387</v>
       </c>
@@ -5341,7 +5347,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="134" spans="1:7">
       <c r="A134" s="3" t="s">
         <v>390</v>
       </c>
@@ -5364,7 +5370,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="135" spans="1:7">
       <c r="A135" s="3" t="s">
         <v>392</v>
       </c>
@@ -5387,7 +5393,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="136" spans="1:7">
       <c r="A136" s="3" t="s">
         <v>395</v>
       </c>
@@ -5410,7 +5416,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="137" spans="1:7">
       <c r="A137" s="3" t="s">
         <v>397</v>
       </c>
@@ -5433,7 +5439,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="138" spans="1:7">
       <c r="A138" s="3" t="s">
         <v>400</v>
       </c>
@@ -5456,7 +5462,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="139" spans="1:7">
       <c r="A139" s="3" t="s">
         <v>403</v>
       </c>
@@ -5479,7 +5485,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="140" spans="1:7">
       <c r="A140" s="3" t="s">
         <v>406</v>
       </c>
@@ -5502,7 +5508,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="141" spans="1:7">
       <c r="A141" s="3" t="s">
         <v>409</v>
       </c>
@@ -5525,7 +5531,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="142" spans="1:7">
       <c r="A142" s="3" t="s">
         <v>411</v>
       </c>
@@ -5548,7 +5554,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="143" spans="1:7">
       <c r="A143" s="3" t="s">
         <v>414</v>
       </c>
@@ -5571,7 +5577,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="144" spans="1:7">
       <c r="A144" s="3" t="s">
         <v>415</v>
       </c>
@@ -5594,7 +5600,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="145" spans="1:7">
       <c r="A145" s="3" t="s">
         <v>418</v>
       </c>
@@ -5617,7 +5623,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="146" spans="1:7">
       <c r="A146" s="3" t="s">
         <v>421</v>
       </c>
@@ -5640,7 +5646,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="147" spans="1:7">
       <c r="A147" s="3" t="s">
         <v>424</v>
       </c>
@@ -5663,7 +5669,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="148" spans="1:7">
       <c r="A148" s="3" t="s">
         <v>427</v>
       </c>
@@ -5686,7 +5692,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="149" spans="1:7">
       <c r="A149" s="3" t="s">
         <v>429</v>
       </c>
@@ -5709,7 +5715,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="150" spans="1:7">
       <c r="A150" s="3" t="s">
         <v>432</v>
       </c>
@@ -5732,7 +5738,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="151" spans="1:7">
       <c r="A151" s="3" t="s">
         <v>434</v>
       </c>
@@ -5755,7 +5761,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="152" spans="1:7">
       <c r="A152" s="3" t="s">
         <v>437</v>
       </c>
@@ -5778,7 +5784,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="153" spans="1:7">
       <c r="A153" s="3" t="s">
         <v>440</v>
       </c>
@@ -5801,7 +5807,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="154" spans="1:7">
       <c r="A154" s="3" t="s">
         <v>442</v>
       </c>
@@ -5824,7 +5830,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="155" spans="1:7">
       <c r="A155" s="3" t="s">
         <v>444</v>
       </c>
@@ -5847,7 +5853,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="156" spans="1:7">
       <c r="A156" s="3" t="s">
         <v>447</v>
       </c>
@@ -5870,7 +5876,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="157" spans="1:7">
       <c r="A157" s="3" t="s">
         <v>450</v>
       </c>
@@ -5893,7 +5899,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="158" spans="1:7">
       <c r="A158" s="3" t="s">
         <v>453</v>
       </c>
@@ -5916,7 +5922,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="159" spans="1:7">
       <c r="A159" s="3" t="s">
         <v>456</v>
       </c>
@@ -5939,7 +5945,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="160" spans="1:7">
       <c r="A160" s="3" t="s">
         <v>459</v>
       </c>
@@ -5962,7 +5968,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="161" spans="1:7">
       <c r="A161" s="3" t="s">
         <v>462</v>
       </c>
@@ -5985,7 +5991,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="162" spans="1:7">
       <c r="A162" s="3" t="s">
         <v>465</v>
       </c>
@@ -6008,7 +6014,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="163" spans="1:7">
       <c r="A163" s="3" t="s">
         <v>467</v>
       </c>
@@ -6031,7 +6037,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="164" spans="1:7">
       <c r="A164" s="3" t="s">
         <v>470</v>
       </c>
@@ -6054,7 +6060,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="165" spans="1:7">
       <c r="A165" s="3" t="s">
         <v>473</v>
       </c>
@@ -6077,7 +6083,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="166" spans="1:7">
       <c r="A166" s="3" t="s">
         <v>475</v>
       </c>
@@ -6100,7 +6106,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="167" spans="1:7">
       <c r="A167" s="3" t="s">
         <v>478</v>
       </c>
@@ -6123,7 +6129,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="168" spans="1:7">
       <c r="A168" s="3" t="s">
         <v>481</v>
       </c>
@@ -6146,7 +6152,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="169" spans="1:7">
       <c r="A169" s="3" t="s">
         <v>483</v>
       </c>
@@ -6169,7 +6175,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="170" spans="1:7">
       <c r="A170" s="3" t="s">
         <v>486</v>
       </c>
@@ -6192,7 +6198,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="171" spans="1:7">
       <c r="A171" s="3" t="s">
         <v>488</v>
       </c>
@@ -6215,7 +6221,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="172" spans="1:7">
       <c r="A172" s="3" t="s">
         <v>491</v>
       </c>
@@ -6238,7 +6244,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="173" spans="1:7">
       <c r="A173" s="3" t="s">
         <v>494</v>
       </c>
@@ -6261,7 +6267,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="174" spans="1:7">
       <c r="A174" s="3" t="s">
         <v>496</v>
       </c>
@@ -6284,7 +6290,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="175" spans="1:7">
       <c r="A175" s="3" t="s">
         <v>499</v>
       </c>
@@ -6307,7 +6313,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="176" spans="1:7">
       <c r="A176" s="3" t="s">
         <v>502</v>
       </c>
@@ -6330,7 +6336,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="177" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="177" spans="1:7">
       <c r="A177" s="3" t="s">
         <v>504</v>
       </c>
@@ -6353,7 +6359,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="178" spans="1:7">
       <c r="A178" s="3" t="s">
         <v>506</v>
       </c>
@@ -6376,7 +6382,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="179" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="179" spans="1:7">
       <c r="A179" s="3" t="s">
         <v>509</v>
       </c>
@@ -6399,7 +6405,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="180" spans="1:7">
       <c r="A180" s="3" t="s">
         <v>512</v>
       </c>
@@ -6422,7 +6428,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="181" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="181" spans="1:7">
       <c r="A181" s="3" t="s">
         <v>515</v>
       </c>
@@ -6445,7 +6451,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="182" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="182" spans="1:7">
       <c r="A182" s="3" t="s">
         <v>518</v>
       </c>
@@ -6468,7 +6474,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="183" spans="1:7">
       <c r="A183" s="3" t="s">
         <v>521</v>
       </c>
@@ -6491,7 +6497,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="184" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="184" spans="1:7">
       <c r="A184" s="3" t="s">
         <v>523</v>
       </c>
@@ -6514,7 +6520,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="185" spans="1:7">
       <c r="A185" s="3" t="s">
         <v>526</v>
       </c>
@@ -6537,15 +6543,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="186" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="186" spans="1:7">
       <c r="A186" s="6">
         <v>627199</v>
       </c>
       <c r="B186" s="6" t="s">
+        <v>529</v>
+      </c>
+      <c r="C186" s="6" t="s">
         <v>530</v>
-      </c>
-      <c r="C186" s="6" t="s">
-        <v>529</v>
       </c>
       <c r="D186" s="6" t="s">
         <v>29</v>
@@ -6560,7 +6566,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="187" spans="1:7">
       <c r="A187" s="6">
         <v>975150</v>
       </c>
@@ -6583,15 +6589,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="188" spans="1:7">
       <c r="A188" s="6">
         <v>118990</v>
       </c>
       <c r="B188" s="6" t="s">
+        <v>532</v>
+      </c>
+      <c r="C188" s="6" t="s">
         <v>533</v>
-      </c>
-      <c r="C188" s="6" t="s">
-        <v>532</v>
       </c>
       <c r="D188" s="6" t="s">
         <v>72</v>
@@ -6606,7 +6612,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="189" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="189" spans="1:7">
       <c r="A189" s="6">
         <v>118423</v>
       </c>
@@ -6629,7 +6635,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="190" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="190" spans="1:7">
       <c r="A190" s="6">
         <v>118512</v>
       </c>
@@ -6652,7 +6658,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="191" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="191" spans="1:7">
       <c r="A191" s="6">
         <v>118512</v>
       </c>
@@ -6675,7 +6681,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="192" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="192" spans="1:7">
       <c r="A192" s="6">
         <v>118512</v>
       </c>
@@ -6698,16 +6704,16 @@
         <v>12</v>
       </c>
     </row>
-    <row r="193" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="193" spans="1:7">
       <c r="A193" s="6">
         <v>118535</v>
       </c>
       <c r="B193" s="6" t="s">
+        <v>536</v>
+      </c>
+      <c r="C193" s="6" t="s">
         <v>537</v>
       </c>
-      <c r="C193" s="6" t="s">
-        <v>536</v>
-      </c>
       <c r="D193" s="6" t="s">
         <v>10</v>
       </c>
@@ -6721,16 +6727,16 @@
         <v>12</v>
       </c>
     </row>
-    <row r="194" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="194" spans="1:7">
       <c r="A194" s="6">
         <v>118535</v>
       </c>
       <c r="B194" s="6" t="s">
+        <v>536</v>
+      </c>
+      <c r="C194" s="6" t="s">
         <v>537</v>
       </c>
-      <c r="C194" s="6" t="s">
-        <v>536</v>
-      </c>
       <c r="D194" s="6" t="s">
         <v>10</v>
       </c>
@@ -6744,7 +6750,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="195" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="195" spans="1:7">
       <c r="A195" s="6">
         <v>118619</v>
       </c>
@@ -6767,15 +6773,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="196" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="196" spans="1:7">
       <c r="A196" s="6">
         <v>118633</v>
       </c>
       <c r="B196" s="6" t="s">
+        <v>539</v>
+      </c>
+      <c r="C196" s="6" t="s">
         <v>540</v>
-      </c>
-      <c r="C196" s="6" t="s">
-        <v>539</v>
       </c>
       <c r="D196" s="6" t="s">
         <v>25</v>
@@ -6790,16 +6796,16 @@
         <v>12</v>
       </c>
     </row>
-    <row r="197" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="197" spans="1:7">
       <c r="A197" s="6">
         <v>118680</v>
       </c>
       <c r="B197" s="6" t="s">
+        <v>541</v>
+      </c>
+      <c r="C197" s="6" t="s">
         <v>542</v>
       </c>
-      <c r="C197" s="6" t="s">
-        <v>541</v>
-      </c>
       <c r="D197" s="6" t="s">
         <v>10</v>
       </c>
@@ -6813,16 +6819,16 @@
         <v>12</v>
       </c>
     </row>
-    <row r="198" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="198" spans="1:7">
       <c r="A198" s="6">
         <v>119074</v>
       </c>
       <c r="B198" s="6" t="s">
+        <v>543</v>
+      </c>
+      <c r="C198" s="6" t="s">
         <v>544</v>
       </c>
-      <c r="C198" s="6" t="s">
-        <v>543</v>
-      </c>
       <c r="D198" s="6" t="s">
         <v>10</v>
       </c>
@@ -6836,15 +6842,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="199" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="199" spans="1:7">
       <c r="A199" s="6">
         <v>119297</v>
       </c>
       <c r="B199" s="6" t="s">
+        <v>545</v>
+      </c>
+      <c r="C199" s="6" t="s">
         <v>546</v>
-      </c>
-      <c r="C199" s="6" t="s">
-        <v>545</v>
       </c>
       <c r="D199" s="6" t="s">
         <v>29</v>
@@ -6859,7 +6865,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="200" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="200" spans="1:7">
       <c r="A200" s="6">
         <v>200343</v>
       </c>
@@ -6882,16 +6888,16 @@
         <v>12</v>
       </c>
     </row>
-    <row r="201" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="201" spans="1:7">
       <c r="A201" s="6">
         <v>700300</v>
       </c>
       <c r="B201" s="6" t="s">
+        <v>548</v>
+      </c>
+      <c r="C201" s="6" t="s">
         <v>549</v>
       </c>
-      <c r="C201" s="6" t="s">
-        <v>548</v>
-      </c>
       <c r="D201" s="6" t="s">
         <v>10</v>
       </c>
@@ -6905,15 +6911,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="202" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="202" spans="1:7">
       <c r="A202" s="6">
         <v>705247</v>
       </c>
       <c r="B202" s="6" t="s">
+        <v>550</v>
+      </c>
+      <c r="C202" s="6" t="s">
         <v>551</v>
-      </c>
-      <c r="C202" s="6" t="s">
-        <v>550</v>
       </c>
       <c r="D202" s="6" t="s">
         <v>10</v>
@@ -6928,7 +6934,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="203" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="203" spans="1:7">
       <c r="A203" s="6">
         <v>709828</v>
       </c>
@@ -6951,15 +6957,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="204" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="204" spans="1:7">
       <c r="A204" s="6">
         <v>724901</v>
       </c>
       <c r="B204" s="6" t="s">
+        <v>553</v>
+      </c>
+      <c r="C204" s="6" t="s">
         <v>554</v>
-      </c>
-      <c r="C204" s="6" t="s">
-        <v>553</v>
       </c>
       <c r="D204" s="6" t="s">
         <v>555</v>
@@ -6974,7 +6980,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="205" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="205" spans="1:7">
       <c r="A205" s="6">
         <v>725469</v>
       </c>
@@ -6997,15 +7003,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="206" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="206" spans="1:7">
       <c r="A206" s="6">
         <v>750251</v>
       </c>
       <c r="B206" s="6" t="s">
+        <v>557</v>
+      </c>
+      <c r="C206" s="6" t="s">
         <v>558</v>
-      </c>
-      <c r="C206" s="6" t="s">
-        <v>557</v>
       </c>
       <c r="D206" s="6" t="s">
         <v>16</v>
@@ -7020,16 +7026,16 @@
         <v>12</v>
       </c>
     </row>
-    <row r="207" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="207" spans="1:7">
       <c r="A207" s="6">
         <v>752164</v>
       </c>
       <c r="B207" s="6" t="s">
+        <v>559</v>
+      </c>
+      <c r="C207" s="6" t="s">
         <v>560</v>
       </c>
-      <c r="C207" s="6" t="s">
-        <v>559</v>
-      </c>
       <c r="D207" s="6" t="s">
         <v>10</v>
       </c>
@@ -7043,16 +7049,16 @@
         <v>12</v>
       </c>
     </row>
-    <row r="208" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="208" spans="1:7">
       <c r="A208" s="6">
         <v>752164</v>
       </c>
       <c r="B208" s="6" t="s">
+        <v>559</v>
+      </c>
+      <c r="C208" s="6" t="s">
         <v>560</v>
       </c>
-      <c r="C208" s="6" t="s">
-        <v>559</v>
-      </c>
       <c r="D208" s="6" t="s">
         <v>10</v>
       </c>
@@ -7066,16 +7072,16 @@
         <v>12</v>
       </c>
     </row>
-    <row r="209" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="209" spans="1:7">
       <c r="A209" s="6">
         <v>752164</v>
       </c>
       <c r="B209" s="6" t="s">
+        <v>559</v>
+      </c>
+      <c r="C209" s="6" t="s">
         <v>560</v>
       </c>
-      <c r="C209" s="6" t="s">
-        <v>559</v>
-      </c>
       <c r="D209" s="6" t="s">
         <v>10</v>
       </c>
@@ -7089,15 +7095,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="210" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="210" spans="1:7">
       <c r="A210" s="6">
         <v>763331</v>
       </c>
       <c r="B210" s="6" t="s">
+        <v>561</v>
+      </c>
+      <c r="C210" s="6" t="s">
         <v>562</v>
-      </c>
-      <c r="C210" s="6" t="s">
-        <v>561</v>
       </c>
       <c r="D210" s="6" t="s">
         <v>10</v>
@@ -7112,15 +7118,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="211" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="211" spans="1:7">
       <c r="A211" s="6">
         <v>763331</v>
       </c>
       <c r="B211" s="6" t="s">
+        <v>561</v>
+      </c>
+      <c r="C211" s="6" t="s">
         <v>562</v>
-      </c>
-      <c r="C211" s="6" t="s">
-        <v>561</v>
       </c>
       <c r="D211" s="6" t="s">
         <v>10</v>
@@ -7135,15 +7141,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="212" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="212" spans="1:7">
       <c r="A212" s="6">
         <v>764963</v>
       </c>
       <c r="B212" s="6" t="s">
+        <v>563</v>
+      </c>
+      <c r="C212" s="6" t="s">
         <v>564</v>
-      </c>
-      <c r="C212" s="6" t="s">
-        <v>563</v>
       </c>
       <c r="D212" s="6" t="s">
         <v>10</v>
@@ -7158,15 +7164,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="213" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="213" spans="1:7">
       <c r="A213" s="6">
         <v>764963</v>
       </c>
       <c r="B213" s="6" t="s">
+        <v>563</v>
+      </c>
+      <c r="C213" s="6" t="s">
         <v>564</v>
-      </c>
-      <c r="C213" s="6" t="s">
-        <v>563</v>
       </c>
       <c r="D213" s="6" t="s">
         <v>10</v>
@@ -7181,15 +7187,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="214" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="214" spans="1:7">
       <c r="A214" s="6">
         <v>764963</v>
       </c>
       <c r="B214" s="6" t="s">
+        <v>563</v>
+      </c>
+      <c r="C214" s="6" t="s">
         <v>564</v>
-      </c>
-      <c r="C214" s="6" t="s">
-        <v>563</v>
       </c>
       <c r="D214" s="6" t="s">
         <v>10</v>
@@ -7204,15 +7210,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="215" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="215" spans="1:7">
       <c r="A215" s="6">
         <v>769657</v>
       </c>
       <c r="B215" s="6" t="s">
+        <v>565</v>
+      </c>
+      <c r="C215" s="6" t="s">
         <v>566</v>
-      </c>
-      <c r="C215" s="6" t="s">
-        <v>565</v>
       </c>
       <c r="D215" s="6" t="s">
         <v>16</v>
@@ -7227,7 +7233,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="216" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="216" spans="1:7">
       <c r="A216" s="6">
         <v>772915</v>
       </c>
@@ -7250,15 +7256,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="217" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="217" spans="1:7">
       <c r="A217" s="6">
         <v>784998</v>
       </c>
       <c r="B217" s="6" t="s">
+        <v>568</v>
+      </c>
+      <c r="C217" s="6" t="s">
         <v>569</v>
-      </c>
-      <c r="C217" s="6" t="s">
-        <v>568</v>
       </c>
       <c r="D217" s="6" t="s">
         <v>25</v>
@@ -7273,15 +7279,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="218" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="218" spans="1:7">
       <c r="A218" s="6">
         <v>784998</v>
       </c>
       <c r="B218" s="6" t="s">
+        <v>568</v>
+      </c>
+      <c r="C218" s="6" t="s">
         <v>569</v>
-      </c>
-      <c r="C218" s="6" t="s">
-        <v>568</v>
       </c>
       <c r="D218" s="6" t="s">
         <v>25</v>
@@ -7296,15 +7302,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="219" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="219" spans="1:7">
       <c r="A219" s="6">
         <v>817615</v>
       </c>
       <c r="B219" s="6" t="s">
+        <v>570</v>
+      </c>
+      <c r="C219" s="6" t="s">
         <v>571</v>
-      </c>
-      <c r="C219" s="6" t="s">
-        <v>570</v>
       </c>
       <c r="D219" s="6" t="s">
         <v>10</v>
@@ -7319,7 +7325,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="220" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="220" spans="1:7">
       <c r="A220" s="6">
         <v>822371</v>
       </c>
@@ -7342,7 +7348,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="221" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="221" spans="1:7">
       <c r="A221" s="6">
         <v>822371</v>
       </c>
@@ -7365,15 +7371,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="222" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="222" spans="1:7">
       <c r="A222" s="6">
         <v>826295</v>
       </c>
       <c r="B222" s="6" t="s">
+        <v>572</v>
+      </c>
+      <c r="C222" s="6" t="s">
         <v>573</v>
-      </c>
-      <c r="C222" s="6" t="s">
-        <v>572</v>
       </c>
       <c r="D222" s="6" t="s">
         <v>10</v>
@@ -7388,15 +7394,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="223" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="223" spans="1:7">
       <c r="A223" s="6">
         <v>840189</v>
       </c>
       <c r="B223" s="6" t="s">
+        <v>574</v>
+      </c>
+      <c r="C223" s="6" t="s">
         <v>575</v>
-      </c>
-      <c r="C223" s="6" t="s">
-        <v>574</v>
       </c>
       <c r="D223" s="6" t="s">
         <v>16</v>
@@ -7411,7 +7417,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="224" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="224" spans="1:7">
       <c r="A224" s="6">
         <v>848012</v>
       </c>
@@ -7419,7 +7425,7 @@
         <v>576</v>
       </c>
       <c r="C224" s="6" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="D224" s="6" t="s">
         <v>10</v>
@@ -7434,7 +7440,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="225" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="225" spans="1:7">
       <c r="A225" s="6">
         <v>848012</v>
       </c>
@@ -7442,7 +7448,7 @@
         <v>576</v>
       </c>
       <c r="C225" s="6" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="D225" s="6" t="s">
         <v>10</v>
@@ -7457,7 +7463,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="226" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="226" spans="1:7">
       <c r="A226" s="6">
         <v>848012</v>
       </c>
@@ -7465,7 +7471,7 @@
         <v>576</v>
       </c>
       <c r="C226" s="6" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="D226" s="6" t="s">
         <v>10</v>
@@ -7480,7 +7486,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="227" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="227" spans="1:7">
       <c r="A227" s="6">
         <v>848012</v>
       </c>
@@ -7488,7 +7494,7 @@
         <v>576</v>
       </c>
       <c r="C227" s="6" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="D227" s="6" t="s">
         <v>10</v>
@@ -7503,15 +7509,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="228" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="228" spans="1:7">
       <c r="A228" s="6">
         <v>848075</v>
       </c>
       <c r="B228" s="6" t="s">
+        <v>577</v>
+      </c>
+      <c r="C228" s="6" t="s">
         <v>578</v>
-      </c>
-      <c r="C228" s="6" t="s">
-        <v>577</v>
       </c>
       <c r="D228" s="6" t="s">
         <v>10</v>
@@ -7526,15 +7532,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="229" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="229" spans="1:7">
       <c r="A229" s="6">
         <v>848075</v>
       </c>
       <c r="B229" s="6" t="s">
+        <v>577</v>
+      </c>
+      <c r="C229" s="6" t="s">
         <v>578</v>
-      </c>
-      <c r="C229" s="6" t="s">
-        <v>577</v>
       </c>
       <c r="D229" s="6" t="s">
         <v>10</v>
@@ -7549,15 +7555,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="230" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="230" spans="1:7">
       <c r="A230" s="6">
         <v>853875</v>
       </c>
       <c r="B230" s="6" t="s">
+        <v>579</v>
+      </c>
+      <c r="C230" s="6" t="s">
         <v>580</v>
-      </c>
-      <c r="C230" s="6" t="s">
-        <v>579</v>
       </c>
       <c r="D230" s="6" t="s">
         <v>29</v>
@@ -7572,7 +7578,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="231" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="231" spans="1:7">
       <c r="A231" s="6">
         <v>865008</v>
       </c>
@@ -7595,7 +7601,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="232" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="232" spans="1:7">
       <c r="A232" s="6">
         <v>869238</v>
       </c>
@@ -7618,7 +7624,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="233" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="233" spans="1:7">
       <c r="A233" s="6">
         <v>869238</v>
       </c>
@@ -7641,15 +7647,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="234" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="234" spans="1:7">
       <c r="A234" s="6">
         <v>877560</v>
       </c>
       <c r="B234" s="6" t="s">
+        <v>583</v>
+      </c>
+      <c r="C234" s="6" t="s">
         <v>584</v>
-      </c>
-      <c r="C234" s="6" t="s">
-        <v>583</v>
       </c>
       <c r="D234" s="6" t="s">
         <v>16</v>
@@ -7664,7 +7670,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="235" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="235" spans="1:7">
       <c r="A235" s="6">
         <v>902833</v>
       </c>
@@ -7687,15 +7693,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="236" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="236" spans="1:7">
       <c r="A236" s="6">
         <v>914725</v>
       </c>
       <c r="B236" s="6" t="s">
+        <v>586</v>
+      </c>
+      <c r="C236" s="6" t="s">
         <v>587</v>
-      </c>
-      <c r="C236" s="6" t="s">
-        <v>586</v>
       </c>
       <c r="D236" s="6" t="s">
         <v>25</v>
@@ -7710,15 +7716,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="237" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="237" spans="1:7">
       <c r="A237" s="6">
         <v>921923</v>
       </c>
       <c r="B237" s="6" t="s">
+        <v>588</v>
+      </c>
+      <c r="C237" s="6" t="s">
         <v>589</v>
-      </c>
-      <c r="C237" s="6" t="s">
-        <v>588</v>
       </c>
       <c r="D237" s="6" t="s">
         <v>25</v>
@@ -7733,15 +7739,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="238" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="238" spans="1:7">
       <c r="A238" s="6">
         <v>930935</v>
       </c>
       <c r="B238" s="6" t="s">
+        <v>590</v>
+      </c>
+      <c r="C238" s="6" t="s">
         <v>591</v>
-      </c>
-      <c r="C238" s="6" t="s">
-        <v>590</v>
       </c>
       <c r="D238" s="6" t="s">
         <v>10</v>
@@ -7756,15 +7762,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="239" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="239" spans="1:7">
       <c r="A239" s="6">
         <v>946622</v>
       </c>
       <c r="B239" s="6" t="s">
+        <v>592</v>
+      </c>
+      <c r="C239" s="6" t="s">
         <v>593</v>
-      </c>
-      <c r="C239" s="6" t="s">
-        <v>592</v>
       </c>
       <c r="D239" s="6" t="s">
         <v>10</v>
@@ -7779,15 +7785,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="240" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="240" spans="1:7">
       <c r="A240" s="6">
         <v>946622</v>
       </c>
       <c r="B240" s="6" t="s">
+        <v>592</v>
+      </c>
+      <c r="C240" s="6" t="s">
         <v>593</v>
-      </c>
-      <c r="C240" s="6" t="s">
-        <v>592</v>
       </c>
       <c r="D240" s="6" t="s">
         <v>10</v>
@@ -7802,15 +7808,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="241" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="241" spans="1:7">
       <c r="A241" s="6">
         <v>967159</v>
       </c>
       <c r="B241" s="6" t="s">
+        <v>594</v>
+      </c>
+      <c r="C241" s="6" t="s">
         <v>595</v>
-      </c>
-      <c r="C241" s="6" t="s">
-        <v>594</v>
       </c>
       <c r="D241" s="6" t="s">
         <v>25</v>
@@ -7825,15 +7831,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="242" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="242" spans="1:7">
       <c r="A242" s="6">
         <v>967159</v>
       </c>
       <c r="B242" s="6" t="s">
+        <v>594</v>
+      </c>
+      <c r="C242" s="6" t="s">
         <v>595</v>
-      </c>
-      <c r="C242" s="6" t="s">
-        <v>594</v>
       </c>
       <c r="D242" s="6" t="s">
         <v>25</v>
@@ -7848,15 +7854,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="243" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="243" spans="1:7">
       <c r="A243" s="6">
         <v>967159</v>
       </c>
       <c r="B243" s="6" t="s">
+        <v>594</v>
+      </c>
+      <c r="C243" s="6" t="s">
         <v>595</v>
-      </c>
-      <c r="C243" s="6" t="s">
-        <v>594</v>
       </c>
       <c r="D243" s="6" t="s">
         <v>25</v>
@@ -7871,7 +7877,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="244" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="244" spans="1:7">
       <c r="A244" s="6">
         <v>978318</v>
       </c>
@@ -7894,7 +7900,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="245" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="245" spans="1:7">
       <c r="A245" s="6">
         <v>978318</v>
       </c>
@@ -7913,8 +7919,11 @@
       <c r="F245" s="6">
         <v>2027</v>
       </c>
-    </row>
-    <row r="246" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="G245" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="246" spans="1:7">
       <c r="A246" s="6">
         <v>978318</v>
       </c>
@@ -7933,8 +7942,11 @@
       <c r="F246" s="6">
         <v>2027</v>
       </c>
-    </row>
-    <row r="247" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="G246" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="247" spans="1:7">
       <c r="A247" s="6">
         <v>978318</v>
       </c>
@@ -7953,8 +7965,11 @@
       <c r="F247" s="6">
         <v>2027</v>
       </c>
-    </row>
-    <row r="248" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="G247" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="248" spans="1:7">
       <c r="A248" s="6">
         <v>978318</v>
       </c>
@@ -7973,8 +7988,11 @@
       <c r="F248" s="6">
         <v>2027</v>
       </c>
-    </row>
-    <row r="249" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="G248" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="249" spans="1:7">
       <c r="A249" s="6">
         <v>996050</v>
       </c>
@@ -7993,8 +8011,11 @@
       <c r="F249" s="6">
         <v>2025</v>
       </c>
-    </row>
-    <row r="250" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="G249" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="250" spans="1:7">
       <c r="A250" s="6">
         <v>996160</v>
       </c>
@@ -8013,8 +8034,11 @@
       <c r="F250" s="6">
         <v>2025</v>
       </c>
-    </row>
-    <row r="251" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="G250" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="251" spans="1:7">
       <c r="A251" s="6">
         <v>999274</v>
       </c>
@@ -8033,8 +8057,11 @@
       <c r="F251" s="6">
         <v>2025</v>
       </c>
-    </row>
-    <row r="252" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="G251" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="252" spans="1:7">
       <c r="A252" s="6">
         <v>999274</v>
       </c>
@@ -8053,8 +8080,11 @@
       <c r="F252" s="6">
         <v>2025</v>
       </c>
-    </row>
-    <row r="253" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="G252" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="253" spans="1:7">
       <c r="A253" s="6">
         <v>999607</v>
       </c>
@@ -8073,17 +8103,20 @@
       <c r="F253" s="6">
         <v>2025</v>
       </c>
-    </row>
-    <row r="254" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="G253" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="254" spans="1:7">
       <c r="A254" s="6">
         <v>999712</v>
       </c>
       <c r="B254" s="6" t="s">
+        <v>601</v>
+      </c>
+      <c r="C254" s="6" t="s">
         <v>602</v>
       </c>
-      <c r="C254" s="6" t="s">
-        <v>601</v>
-      </c>
       <c r="D254" s="6" t="s">
         <v>10</v>
       </c>
@@ -8093,17 +8126,20 @@
       <c r="F254" s="6">
         <v>2025</v>
       </c>
-    </row>
-    <row r="255" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="G254" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="255" spans="1:7">
       <c r="A255" s="6">
         <v>999712</v>
       </c>
       <c r="B255" s="6" t="s">
+        <v>601</v>
+      </c>
+      <c r="C255" s="6" t="s">
         <v>602</v>
       </c>
-      <c r="C255" s="6" t="s">
-        <v>601</v>
-      </c>
       <c r="D255" s="6" t="s">
         <v>10</v>
       </c>
@@ -8113,17 +8149,20 @@
       <c r="F255" s="6">
         <v>2025</v>
       </c>
-    </row>
-    <row r="256" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="G255" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="256" spans="1:7">
       <c r="A256" s="6">
         <v>999712</v>
       </c>
       <c r="B256" s="6" t="s">
+        <v>601</v>
+      </c>
+      <c r="C256" s="6" t="s">
         <v>602</v>
       </c>
-      <c r="C256" s="6" t="s">
-        <v>601</v>
-      </c>
       <c r="D256" s="6" t="s">
         <v>10</v>
       </c>
@@ -8133,10 +8172,77 @@
       <c r="F256" s="6">
         <v>2025</v>
       </c>
-    </row>
-    <row r="257" spans="5:5" x14ac:dyDescent="0.15">
+      <c r="G256" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="257" spans="1:7">
+      <c r="A257" s="6">
+        <v>999003</v>
+      </c>
+      <c r="B257" s="6" t="s">
+        <v>603</v>
+      </c>
+      <c r="C257" s="6" t="s">
+        <v>604</v>
+      </c>
+      <c r="D257" s="6" t="s">
+        <v>10</v>
+      </c>
       <c r="E257" s="3" t="s">
         <v>11</v>
+      </c>
+      <c r="F257" s="6">
+        <v>2025</v>
+      </c>
+      <c r="G257" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="258" spans="1:7">
+      <c r="A258" s="6">
+        <v>119413</v>
+      </c>
+      <c r="B258" s="6" t="s">
+        <v>388</v>
+      </c>
+      <c r="C258" s="6" t="s">
+        <v>389</v>
+      </c>
+      <c r="D258" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E258" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F258" s="6">
+        <v>2025</v>
+      </c>
+      <c r="G258" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="259" spans="1:7">
+      <c r="A259" s="6">
+        <v>999010</v>
+      </c>
+      <c r="B259" s="6" t="s">
+        <v>340</v>
+      </c>
+      <c r="C259" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="D259" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E259" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F259" s="6">
+        <v>2025</v>
+      </c>
+      <c r="G259" s="6" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -8411,40 +8517,13 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A5E07700-420E-46F7-9DE6-7AF35B4B035E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="efce84db-8738-4c7b-9bdc-65b9500871f6"/>
-    <ds:schemaRef ds:uri="e4ac40dc-80da-4869-807e-191aa97932d8"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A5E07700-420E-46F7-9DE6-7AF35B4B035E}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C1B82C93-0C8A-42A6-94D3-03BD21DA2B68}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C1B82C93-0C8A-42A6-94D3-03BD21DA2B68}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{506B5D65-D17D-4B19-A762-8B542DECFC4D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="e4ac40dc-80da-4869-807e-191aa97932d8"/>
-    <ds:schemaRef ds:uri="c8e8eaa7-2320-4408-9564-9ed5178ae212"/>
-    <ds:schemaRef ds:uri="efce84db-8738-4c7b-9bdc-65b9500871f6"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{506B5D65-D17D-4B19-A762-8B542DECFC4D}"/>
 </file>
</xml_diff>